<commit_message>
Adding a R project file and filling in missing data with the data from frequency tables - all freq tables bounds have been added and the numbers all double checked
</commit_message>
<xml_diff>
--- a/PowerEstimationReviewDataCollection2018.03.25.xlsx
+++ b/PowerEstimationReviewDataCollection2018.03.25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Systematic Reviews\History of Power Estimation Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70955A6-D15D-4308-BCD2-938EC521FD63}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C0F6D8-B6E9-4AD0-877F-BD1819DC3FCD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="10640" windowHeight="5720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,6 +32,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="1217">
   <si>
     <t>Author</t>
   </si>
@@ -3750,13 +3755,16 @@
     <t xml:space="preserve">1 if sds were estimated from frequency tables and not reported directly </t>
   </si>
   <si>
-    <t>SDSmallEstimatedFromCDT</t>
-  </si>
-  <si>
     <t>Note, SDs had to be calculated manually from raw sds for the two types of tests (i.e., t tests and f tests)</t>
   </si>
   <si>
-    <t>!!!!!!!</t>
+    <t>SDSmallAlgEstFromCDT</t>
+  </si>
+  <si>
+    <t>SDMedAlgEstFromCDT</t>
+  </si>
+  <si>
+    <t>SDLargeAlgEstFromCDT</t>
   </si>
 </sst>
 </file>
@@ -4234,11 +4242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG128"/>
+  <dimension ref="A1:BI128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="38" zoomScaleNormal="47" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" zoomScale="31" zoomScaleNormal="47" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -4269,15 +4277,15 @@
     <col min="28" max="32" width="10.83203125" style="7" customWidth="1"/>
     <col min="33" max="35" width="10.83203125" style="1" customWidth="1"/>
     <col min="36" max="36" width="10.83203125" style="9" customWidth="1"/>
-    <col min="37" max="41" width="10.83203125" style="1" customWidth="1"/>
-    <col min="42" max="42" width="10.83203125" style="1"/>
-    <col min="43" max="51" width="10.83203125" style="1" customWidth="1"/>
-    <col min="52" max="57" width="10.83203125" style="1"/>
-    <col min="58" max="58" width="41.9140625" style="1" customWidth="1"/>
-    <col min="59" max="16384" width="10.83203125" style="1"/>
+    <col min="37" max="43" width="10.83203125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="10.83203125" style="1"/>
+    <col min="45" max="53" width="10.83203125" style="1" customWidth="1"/>
+    <col min="54" max="59" width="10.83203125" style="1"/>
+    <col min="60" max="60" width="41.9140625" style="1" customWidth="1"/>
+    <col min="61" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59">
+    <row r="1" spans="1:61">
       <c r="A1" s="1" t="s">
         <v>414</v>
       </c>
@@ -4399,58 +4407,64 @@
         <v>400</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="AP1" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>1110</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>1111</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>1112</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>1113</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>1114</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>1115</v>
       </c>
     </row>
-    <row r="2" spans="1:59">
+    <row r="2" spans="1:61">
       <c r="A2" s="1">
         <v>100</v>
       </c>
@@ -4469,15 +4483,15 @@
       <c r="F2" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="AT2" s="4"/>
-      <c r="BB2" s="1">
+      <c r="AV2" s="4"/>
+      <c r="BD2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:59">
+    <row r="3" spans="1:61">
       <c r="A3" s="1">
         <v>49</v>
       </c>
@@ -4565,9 +4579,9 @@
       <c r="AJ3" s="9">
         <v>146</v>
       </c>
-      <c r="AT3" s="4"/>
-    </row>
-    <row r="4" spans="1:59">
+      <c r="AV3" s="4"/>
+    </row>
+    <row r="4" spans="1:61">
       <c r="A4" s="1">
         <v>49</v>
       </c>
@@ -4631,9 +4645,9 @@
       <c r="AF4" s="7">
         <v>0.69699999999999995</v>
       </c>
-      <c r="AT4" s="4"/>
-    </row>
-    <row r="5" spans="1:59">
+      <c r="AV4" s="4"/>
+    </row>
+    <row r="5" spans="1:61">
       <c r="A5" s="7">
         <v>60</v>
       </c>
@@ -4736,13 +4750,13 @@
       <c r="AN5" s="1">
         <v>116.84</v>
       </c>
-      <c r="AP5" s="1" t="s">
+      <c r="AR5" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="AT5" s="4"/>
-      <c r="BG5" s="7"/>
-    </row>
-    <row r="6" spans="1:59">
+      <c r="AV5" s="4"/>
+      <c r="BI5" s="7"/>
+    </row>
+    <row r="6" spans="1:61">
       <c r="A6" s="1">
         <v>77</v>
       </c>
@@ -4836,12 +4850,12 @@
       <c r="AL6" s="1">
         <v>386</v>
       </c>
-      <c r="AP6" s="7" t="s">
+      <c r="AR6" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="AT6" s="4"/>
-    </row>
-    <row r="7" spans="1:59">
+      <c r="AV6" s="4"/>
+    </row>
+    <row r="7" spans="1:61">
       <c r="A7" s="1">
         <v>77</v>
       </c>
@@ -4923,10 +4937,10 @@
       <c r="AL7" s="1">
         <v>206</v>
       </c>
-      <c r="AP7" s="4"/>
-      <c r="AT7" s="4"/>
-    </row>
-    <row r="8" spans="1:59">
+      <c r="AR7" s="4"/>
+      <c r="AV7" s="4"/>
+    </row>
+    <row r="8" spans="1:61">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -5008,10 +5022,10 @@
       <c r="AL8" s="1">
         <v>39</v>
       </c>
-      <c r="AP8" s="4"/>
-      <c r="AT8" s="4"/>
-    </row>
-    <row r="9" spans="1:59">
+      <c r="AR8" s="4"/>
+      <c r="AV8" s="4"/>
+    </row>
+    <row r="9" spans="1:61">
       <c r="A9" s="1">
         <v>77</v>
       </c>
@@ -5093,10 +5107,10 @@
       <c r="AL9" s="1">
         <v>124</v>
       </c>
-      <c r="AP9" s="4"/>
-      <c r="AT9" s="4"/>
-    </row>
-    <row r="10" spans="1:59">
+      <c r="AR9" s="4"/>
+      <c r="AV9" s="4"/>
+    </row>
+    <row r="10" spans="1:61">
       <c r="A10" s="1">
         <v>77</v>
       </c>
@@ -5178,10 +5192,10 @@
       <c r="AL10" s="1">
         <v>85</v>
       </c>
-      <c r="AP10" s="4"/>
-      <c r="AT10" s="4"/>
-    </row>
-    <row r="11" spans="1:59">
+      <c r="AR10" s="4"/>
+      <c r="AV10" s="4"/>
+    </row>
+    <row r="11" spans="1:61">
       <c r="A11" s="1">
         <v>69</v>
       </c>
@@ -5257,23 +5271,23 @@
       <c r="Z11" s="7">
         <v>0.53600000000000003</v>
       </c>
-      <c r="AP11" s="1" t="s">
+      <c r="AR11" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="AT11" s="4">
+      <c r="AV11" s="4">
         <v>0.05</v>
       </c>
-      <c r="AU11" s="1">
+      <c r="AW11" s="1">
         <v>1</v>
       </c>
-      <c r="AV11" s="1">
+      <c r="AX11" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AW11" s="1">
+      <c r="AY11" s="1">
         <v>0.996</v>
       </c>
     </row>
-    <row r="12" spans="1:59">
+    <row r="12" spans="1:61">
       <c r="A12" s="1">
         <v>69</v>
       </c>
@@ -5343,23 +5357,23 @@
       <c r="Z12" s="7">
         <v>0.159</v>
       </c>
-      <c r="AP12" s="1" t="s">
+      <c r="AR12" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="AT12" s="1">
+      <c r="AV12" s="1">
         <v>0.05</v>
       </c>
-      <c r="AU12" s="1">
+      <c r="AW12" s="1">
         <v>0.82699999999999996</v>
       </c>
-      <c r="AV12" s="1">
+      <c r="AX12" s="1">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="AW12" s="1">
+      <c r="AY12" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:59">
+    <row r="13" spans="1:61">
       <c r="A13" s="1">
         <v>69</v>
       </c>
@@ -5429,23 +5443,23 @@
       <c r="Z13" s="7">
         <v>0.997</v>
       </c>
-      <c r="AP13" s="1" t="s">
+      <c r="AR13" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="AT13" s="1">
+      <c r="AV13" s="1">
         <v>0.05</v>
       </c>
-      <c r="AU13" s="1">
+      <c r="AW13" s="1">
         <v>0.89419999999999999</v>
       </c>
-      <c r="AV13" s="1">
+      <c r="AX13" s="1">
         <v>5.1400000000000001E-2</v>
       </c>
-      <c r="AW13" s="1">
+      <c r="AY13" s="1">
         <v>0.997</v>
       </c>
     </row>
-    <row r="14" spans="1:59">
+    <row r="14" spans="1:61">
       <c r="A14" s="1">
         <v>109</v>
       </c>
@@ -5509,14 +5523,14 @@
       <c r="AJ14" s="9">
         <v>43</v>
       </c>
-      <c r="AP14" s="1" t="s">
+      <c r="AR14" s="1" t="s">
         <v>1178</v>
       </c>
-      <c r="BB14" s="1">
+      <c r="BD14" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:59">
+    <row r="15" spans="1:61">
       <c r="A15" s="1">
         <v>46</v>
       </c>
@@ -5535,14 +5549,14 @@
       <c r="F15" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="AP15" s="1" t="s">
+      <c r="AR15" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="AZ15" s="1">
+      <c r="BB15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:59">
+    <row r="16" spans="1:61">
       <c r="A16" s="1">
         <v>84</v>
       </c>
@@ -5561,14 +5575,14 @@
       <c r="F16" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="AP16" s="1" t="s">
+      <c r="AR16" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="BB16" s="1">
+      <c r="BD16" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:59">
+    <row r="17" spans="1:61">
       <c r="A17" s="1">
         <v>63</v>
       </c>
@@ -5623,14 +5637,14 @@
       <c r="X17" s="9">
         <v>0.18</v>
       </c>
-      <c r="AP17" s="1" t="s">
+      <c r="AR17" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="BB17" s="1">
+      <c r="BD17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:59">
+    <row r="18" spans="1:61">
       <c r="A18" s="1">
         <v>74</v>
       </c>
@@ -5718,11 +5732,11 @@
       <c r="AC18" s="7">
         <v>1</v>
       </c>
-      <c r="BE18" s="1">
+      <c r="BG18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:59">
+    <row r="19" spans="1:61">
       <c r="A19" s="1">
         <v>107</v>
       </c>
@@ -5835,7 +5849,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:59">
+    <row r="20" spans="1:61">
       <c r="A20" s="1">
         <v>71</v>
       </c>
@@ -5953,11 +5967,11 @@
       <c r="AN20" s="1">
         <v>44.45</v>
       </c>
-      <c r="AP20" s="1" t="s">
+      <c r="AR20" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="21" spans="1:59">
+    <row r="21" spans="1:61">
       <c r="A21" s="1">
         <v>113</v>
       </c>
@@ -6018,14 +6032,14 @@
       <c r="AJ21" s="9">
         <v>16</v>
       </c>
-      <c r="AP21" s="1" t="s">
+      <c r="AR21" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="BD21" s="1">
+      <c r="BF21" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:59">
+    <row r="22" spans="1:61">
       <c r="A22" s="1">
         <v>66</v>
       </c>
@@ -6104,11 +6118,11 @@
       <c r="AI22" s="1">
         <v>0.13</v>
       </c>
-      <c r="AP22" s="1" t="s">
+      <c r="AR22" s="1" t="s">
         <v>1204</v>
       </c>
     </row>
-    <row r="23" spans="1:59">
+    <row r="23" spans="1:61">
       <c r="A23" s="1">
         <v>53</v>
       </c>
@@ -6127,14 +6141,14 @@
       <c r="F23" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="AP23" s="1" t="s">
+      <c r="AR23" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="BB23" s="1">
+      <c r="BD23" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:59">
+    <row r="24" spans="1:61">
       <c r="A24" s="1">
         <v>75</v>
       </c>
@@ -6219,11 +6233,11 @@
       <c r="AI24" s="1">
         <v>0.19</v>
       </c>
-      <c r="AP24" s="1" t="s">
+      <c r="AR24" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="1:59">
+    <row r="25" spans="1:61">
       <c r="A25" s="1">
         <v>54</v>
       </c>
@@ -6263,14 +6277,14 @@
       <c r="N25" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AP25" s="1" t="s">
+      <c r="AR25" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="BB25" s="1">
+      <c r="BD25" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:59">
+    <row r="26" spans="1:61">
       <c r="A26" s="11">
         <v>102</v>
       </c>
@@ -6370,12 +6384,12 @@
       <c r="AH26" s="1">
         <v>0.23799999999999999</v>
       </c>
-      <c r="AI26" s="1" t="s">
-        <v>1215</v>
-      </c>
-      <c r="BG26" s="11"/>
-    </row>
-    <row r="27" spans="1:59">
+      <c r="AI26" s="1">
+        <v>167</v>
+      </c>
+      <c r="BI26" s="11"/>
+    </row>
+    <row r="27" spans="1:61">
       <c r="A27" s="11">
         <v>90</v>
       </c>
@@ -6406,16 +6420,16 @@
       <c r="T27" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="AP27" s="1" t="s">
+      <c r="AR27" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="BC27" s="1">
+      <c r="BE27" s="1">
         <v>1</v>
       </c>
-      <c r="BF27" s="7"/>
-      <c r="BG27" s="11"/>
-    </row>
-    <row r="28" spans="1:59">
+      <c r="BH27" s="7"/>
+      <c r="BI27" s="11"/>
+    </row>
+    <row r="28" spans="1:61">
       <c r="A28" s="11">
         <v>61</v>
       </c>
@@ -6449,16 +6463,16 @@
       <c r="T28" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="AP28" s="1" t="s">
+      <c r="AR28" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="BB28" s="1">
+      <c r="BD28" s="1">
         <v>1</v>
       </c>
-      <c r="BF28" s="7"/>
-      <c r="BG28" s="11"/>
-    </row>
-    <row r="29" spans="1:59">
+      <c r="BH28" s="7"/>
+      <c r="BI28" s="11"/>
+    </row>
+    <row r="29" spans="1:61">
       <c r="A29" s="11">
         <v>86</v>
       </c>
@@ -6543,9 +6557,9 @@
       <c r="AI29" s="1">
         <v>0.18</v>
       </c>
-      <c r="BG29" s="11"/>
-    </row>
-    <row r="30" spans="1:59">
+      <c r="BI29" s="11"/>
+    </row>
+    <row r="30" spans="1:61">
       <c r="A30" s="11">
         <v>57</v>
       </c>
@@ -6612,16 +6626,16 @@
       <c r="AJ30" s="9">
         <v>86.5</v>
       </c>
-      <c r="AP30" s="1" t="s">
+      <c r="AR30" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="BB30" s="1">
+      <c r="BD30" s="1">
         <v>1</v>
       </c>
-      <c r="BF30" s="7"/>
-      <c r="BG30" s="11"/>
-    </row>
-    <row r="31" spans="1:59">
+      <c r="BH30" s="7"/>
+      <c r="BI30" s="11"/>
+    </row>
+    <row r="31" spans="1:61">
       <c r="A31" s="11">
         <v>57</v>
       </c>
@@ -6682,13 +6696,13 @@
       <c r="AJ31" s="9">
         <v>178.1</v>
       </c>
-      <c r="AP31" s="1" t="s">
+      <c r="AR31" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="BF31" s="7"/>
-      <c r="BG31" s="11"/>
-    </row>
-    <row r="32" spans="1:59">
+      <c r="BH31" s="7"/>
+      <c r="BI31" s="11"/>
+    </row>
+    <row r="32" spans="1:61">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -6750,13 +6764,13 @@
       <c r="AJ32" s="9">
         <v>90.1</v>
       </c>
-      <c r="AP32" s="1" t="s">
+      <c r="AR32" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="BF32" s="7"/>
-      <c r="BG32" s="11"/>
-    </row>
-    <row r="33" spans="1:59">
+      <c r="BH32" s="7"/>
+      <c r="BI32" s="11"/>
+    </row>
+    <row r="33" spans="1:61">
       <c r="A33" s="11">
         <v>57</v>
       </c>
@@ -6818,13 +6832,13 @@
       <c r="AJ33" s="9">
         <v>129</v>
       </c>
-      <c r="AP33" s="1" t="s">
+      <c r="AR33" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="BF33" s="7"/>
-      <c r="BG33" s="11"/>
-    </row>
-    <row r="34" spans="1:59">
+      <c r="BH33" s="7"/>
+      <c r="BI33" s="11"/>
+    </row>
+    <row r="34" spans="1:61">
       <c r="A34" s="11">
         <v>57</v>
       </c>
@@ -6886,13 +6900,13 @@
       <c r="AJ34" s="9">
         <v>94.6</v>
       </c>
-      <c r="AP34" s="1" t="s">
+      <c r="AR34" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="BF34" s="7"/>
-      <c r="BG34" s="11"/>
-    </row>
-    <row r="35" spans="1:59">
+      <c r="BH34" s="7"/>
+      <c r="BI34" s="11"/>
+    </row>
+    <row r="35" spans="1:61">
       <c r="A35" s="11">
         <v>57</v>
       </c>
@@ -6954,13 +6968,13 @@
       <c r="AJ35" s="9">
         <v>72.8</v>
       </c>
-      <c r="AP35" s="1" t="s">
+      <c r="AR35" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="BF35" s="7"/>
-      <c r="BG35" s="11"/>
-    </row>
-    <row r="36" spans="1:59">
+      <c r="BH35" s="7"/>
+      <c r="BI35" s="11"/>
+    </row>
+    <row r="36" spans="1:61">
       <c r="A36" s="11">
         <v>78</v>
       </c>
@@ -7031,16 +7045,16 @@
       <c r="AN36" s="1">
         <v>5654.47</v>
       </c>
-      <c r="AP36" s="1" t="s">
+      <c r="AR36" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="BD36" s="1">
+      <c r="BF36" s="1">
         <v>1</v>
       </c>
-      <c r="BF36" s="7"/>
-      <c r="BG36" s="11"/>
-    </row>
-    <row r="37" spans="1:59">
+      <c r="BH36" s="7"/>
+      <c r="BI36" s="11"/>
+    </row>
+    <row r="37" spans="1:61">
       <c r="A37" s="11">
         <v>64</v>
       </c>
@@ -7098,16 +7112,16 @@
       <c r="T37" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="AP37" s="1" t="s">
+      <c r="AR37" s="1" t="s">
         <v>1179</v>
       </c>
-      <c r="BB37" s="1">
+      <c r="BD37" s="1">
         <v>1</v>
       </c>
-      <c r="BF37" s="7"/>
-      <c r="BG37" s="11"/>
-    </row>
-    <row r="38" spans="1:59">
+      <c r="BH37" s="7"/>
+      <c r="BI37" s="11"/>
+    </row>
+    <row r="38" spans="1:61">
       <c r="A38" s="11">
         <v>68</v>
       </c>
@@ -7225,9 +7239,9 @@
       <c r="AN38" s="1">
         <v>75.2</v>
       </c>
-      <c r="BG38" s="11"/>
-    </row>
-    <row r="39" spans="1:59">
+      <c r="BI38" s="11"/>
+    </row>
+    <row r="39" spans="1:61">
       <c r="A39" s="11">
         <v>93</v>
       </c>
@@ -7288,16 +7302,16 @@
       <c r="AL39" s="1">
         <v>47</v>
       </c>
-      <c r="AP39" s="1" t="s">
+      <c r="AR39" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="BB39" s="1">
+      <c r="BD39" s="1">
         <v>1</v>
       </c>
-      <c r="BF39" s="7"/>
-      <c r="BG39" s="11"/>
-    </row>
-    <row r="40" spans="1:59">
+      <c r="BH39" s="7"/>
+      <c r="BI39" s="11"/>
+    </row>
+    <row r="40" spans="1:61">
       <c r="A40" s="11">
         <v>48</v>
       </c>
@@ -7355,16 +7369,16 @@
       <c r="AL40" s="1">
         <v>53</v>
       </c>
-      <c r="AP40" s="1" t="s">
+      <c r="AR40" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="BD40" s="1">
+      <c r="BF40" s="1">
         <v>1</v>
       </c>
-      <c r="BF40" s="7"/>
-      <c r="BG40" s="11"/>
-    </row>
-    <row r="41" spans="1:59">
+      <c r="BH40" s="7"/>
+      <c r="BI40" s="11"/>
+    </row>
+    <row r="41" spans="1:61">
       <c r="A41" s="11">
         <v>48</v>
       </c>
@@ -7407,10 +7421,10 @@
       <c r="T41" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="BF41" s="7"/>
-      <c r="BG41" s="11"/>
-    </row>
-    <row r="42" spans="1:59" s="11" customFormat="1">
+      <c r="BH41" s="7"/>
+      <c r="BI41" s="11"/>
+    </row>
+    <row r="42" spans="1:61" s="11" customFormat="1">
       <c r="A42" s="11">
         <v>88</v>
       </c>
@@ -7512,7 +7526,7 @@
       </c>
       <c r="AJ42" s="14"/>
     </row>
-    <row r="43" spans="1:59" s="11" customFormat="1">
+    <row r="43" spans="1:61" s="11" customFormat="1">
       <c r="A43" s="11">
         <v>111</v>
       </c>
@@ -7568,14 +7582,16 @@
         <v>413</v>
       </c>
       <c r="AO43" s="12"/>
-      <c r="AP43" s="11" t="s">
+      <c r="AP43" s="12"/>
+      <c r="AQ43" s="12"/>
+      <c r="AR43" s="11" t="s">
         <v>591</v>
       </c>
-      <c r="BD43" s="11">
+      <c r="BF43" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:59" s="11" customFormat="1">
+    <row r="44" spans="1:61" s="11" customFormat="1">
       <c r="A44" s="11">
         <v>111</v>
       </c>
@@ -7625,8 +7641,10 @@
         <v>782</v>
       </c>
       <c r="AO44" s="12"/>
-    </row>
-    <row r="45" spans="1:59" s="11" customFormat="1">
+      <c r="AP44" s="12"/>
+      <c r="AQ44" s="12"/>
+    </row>
+    <row r="45" spans="1:61" s="11" customFormat="1">
       <c r="A45" s="11">
         <v>111</v>
       </c>
@@ -7676,8 +7694,10 @@
         <v>1041</v>
       </c>
       <c r="AO45" s="13"/>
-    </row>
-    <row r="46" spans="1:59" s="11" customFormat="1">
+      <c r="AP45" s="13"/>
+      <c r="AQ45" s="13"/>
+    </row>
+    <row r="46" spans="1:61" s="11" customFormat="1">
       <c r="A46" s="11">
         <v>111</v>
       </c>
@@ -7727,8 +7747,10 @@
         <v>671</v>
       </c>
       <c r="AO46" s="12"/>
-    </row>
-    <row r="47" spans="1:59" s="11" customFormat="1">
+      <c r="AP46" s="12"/>
+      <c r="AQ46" s="12"/>
+    </row>
+    <row r="47" spans="1:61" s="11" customFormat="1">
       <c r="A47" s="11">
         <v>111</v>
       </c>
@@ -7778,8 +7800,10 @@
         <v>309</v>
       </c>
       <c r="AO47" s="12"/>
-    </row>
-    <row r="48" spans="1:59" s="11" customFormat="1">
+      <c r="AP47" s="12"/>
+      <c r="AQ47" s="12"/>
+    </row>
+    <row r="48" spans="1:61" s="11" customFormat="1">
       <c r="A48" s="11">
         <v>56</v>
       </c>
@@ -7802,14 +7826,14 @@
       <c r="X48" s="14"/>
       <c r="AA48" s="14"/>
       <c r="AJ48" s="14"/>
-      <c r="AP48" s="11" t="s">
+      <c r="AR48" s="11" t="s">
         <v>597</v>
       </c>
-      <c r="BD48" s="11">
+      <c r="BF48" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:59" s="11" customFormat="1">
+    <row r="49" spans="1:61" s="11" customFormat="1">
       <c r="A49" s="11">
         <v>82</v>
       </c>
@@ -7832,14 +7856,14 @@
       <c r="X49" s="14"/>
       <c r="AA49" s="14"/>
       <c r="AJ49" s="14"/>
-      <c r="AP49" s="11" t="s">
+      <c r="AR49" s="11" t="s">
         <v>1035</v>
       </c>
-      <c r="BD49" s="11">
+      <c r="BF49" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:59" s="11" customFormat="1">
+    <row r="50" spans="1:61" s="11" customFormat="1">
       <c r="A50" s="11">
         <v>104</v>
       </c>
@@ -7926,7 +7950,7 @@
       </c>
       <c r="AJ50" s="14"/>
     </row>
-    <row r="51" spans="1:59" s="11" customFormat="1">
+    <row r="51" spans="1:61" s="11" customFormat="1">
       <c r="A51" s="11">
         <v>87</v>
       </c>
@@ -7949,14 +7973,14 @@
       <c r="X51" s="14"/>
       <c r="AA51" s="14"/>
       <c r="AJ51" s="14"/>
-      <c r="AP51" s="11" t="s">
+      <c r="AR51" s="11" t="s">
         <v>602</v>
       </c>
-      <c r="BA51" s="11">
+      <c r="BC51" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:59" s="11" customFormat="1">
+    <row r="52" spans="1:61" s="11" customFormat="1">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -8047,11 +8071,11 @@
       <c r="AN52" s="11">
         <v>548</v>
       </c>
-      <c r="AP52" s="7" t="s">
+      <c r="AR52" s="7" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="53" spans="1:59" s="11" customFormat="1">
+    <row r="53" spans="1:61" s="11" customFormat="1">
       <c r="A53" s="11">
         <v>67</v>
       </c>
@@ -8163,8 +8187,10 @@
       <c r="AP53" s="1"/>
       <c r="AQ53" s="1"/>
       <c r="AR53" s="1"/>
-    </row>
-    <row r="54" spans="1:59">
+      <c r="AS53" s="1"/>
+      <c r="AT53" s="1"/>
+    </row>
+    <row r="54" spans="1:61">
       <c r="A54" s="11">
         <v>96</v>
       </c>
@@ -8231,18 +8257,18 @@
       <c r="AE54" s="9">
         <v>0.81</v>
       </c>
-      <c r="AG54" s="1">
-        <v>0.323604</v>
-      </c>
-      <c r="AO54" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP54" s="1" t="s">
+      <c r="AG54" s="26">
+        <v>0.3251309</v>
+      </c>
+      <c r="AO54" s="26">
+        <v>0.3251309</v>
+      </c>
+      <c r="AR54" s="1" t="s">
         <v>1174</v>
       </c>
-      <c r="BG54" s="11"/>
-    </row>
-    <row r="55" spans="1:59">
+      <c r="BI54" s="11"/>
+    </row>
+    <row r="55" spans="1:61">
       <c r="A55" s="11">
         <v>98</v>
       </c>
@@ -8318,9 +8344,9 @@
       <c r="AH55" s="1">
         <v>0.12</v>
       </c>
-      <c r="BG55" s="11"/>
-    </row>
-    <row r="56" spans="1:59">
+      <c r="BI55" s="11"/>
+    </row>
+    <row r="56" spans="1:61">
       <c r="A56" s="11">
         <v>79</v>
       </c>
@@ -8375,19 +8401,19 @@
       <c r="AN56" s="1">
         <v>193.86</v>
       </c>
-      <c r="AR56" s="1">
+      <c r="AT56" s="1">
         <v>1</v>
       </c>
-      <c r="AS56" s="1">
+      <c r="AU56" s="1">
         <v>16584</v>
       </c>
-      <c r="BD56" s="1">
+      <c r="BF56" s="1">
         <v>1</v>
       </c>
-      <c r="BF56" s="7"/>
-      <c r="BG56" s="11"/>
-    </row>
-    <row r="57" spans="1:59">
+      <c r="BH56" s="7"/>
+      <c r="BI56" s="11"/>
+    </row>
+    <row r="57" spans="1:61">
       <c r="A57" s="11">
         <v>79</v>
       </c>
@@ -8436,16 +8462,16 @@
       <c r="AN57" s="1">
         <v>2026.53</v>
       </c>
-      <c r="AR57" s="1">
+      <c r="AT57" s="1">
         <v>1</v>
       </c>
-      <c r="AS57" s="1">
+      <c r="AU57" s="1">
         <v>45144</v>
       </c>
-      <c r="BF57" s="7"/>
-      <c r="BG57" s="11"/>
-    </row>
-    <row r="58" spans="1:59">
+      <c r="BH57" s="7"/>
+      <c r="BI57" s="11"/>
+    </row>
+    <row r="58" spans="1:61">
       <c r="A58" s="11">
         <v>79</v>
       </c>
@@ -8494,16 +8520,16 @@
       <c r="AN58" s="1">
         <v>983.38</v>
       </c>
-      <c r="AR58" s="1">
+      <c r="AT58" s="1">
         <v>1</v>
       </c>
-      <c r="AS58" s="1">
+      <c r="AU58" s="1">
         <v>16930</v>
       </c>
-      <c r="BF58" s="7"/>
-      <c r="BG58" s="11"/>
-    </row>
-    <row r="59" spans="1:59">
+      <c r="BH58" s="7"/>
+      <c r="BI58" s="11"/>
+    </row>
+    <row r="59" spans="1:61">
       <c r="A59" s="11">
         <v>79</v>
       </c>
@@ -8552,16 +8578,16 @@
       <c r="AN59" s="1">
         <v>680.02</v>
       </c>
-      <c r="AR59" s="1">
+      <c r="AT59" s="1">
         <v>1</v>
       </c>
-      <c r="AS59" s="1">
+      <c r="AU59" s="1">
         <v>13059</v>
       </c>
-      <c r="BF59" s="7"/>
-      <c r="BG59" s="11"/>
-    </row>
-    <row r="60" spans="1:59">
+      <c r="BH59" s="7"/>
+      <c r="BI59" s="11"/>
+    </row>
+    <row r="60" spans="1:61">
       <c r="A60" s="11">
         <v>41</v>
       </c>
@@ -8610,16 +8636,16 @@
       <c r="AM60" s="1">
         <v>52</v>
       </c>
-      <c r="AP60" s="1" t="s">
+      <c r="AR60" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="BD60" s="1">
+      <c r="BF60" s="1">
         <v>1</v>
       </c>
-      <c r="BF60" s="7"/>
-      <c r="BG60" s="11"/>
-    </row>
-    <row r="61" spans="1:59">
+      <c r="BH60" s="7"/>
+      <c r="BI60" s="11"/>
+    </row>
+    <row r="61" spans="1:61">
       <c r="A61" s="7">
         <v>41</v>
       </c>
@@ -8662,13 +8688,13 @@
       <c r="AM61" s="1">
         <v>59</v>
       </c>
-      <c r="AP61" s="1" t="s">
+      <c r="AR61" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="BF61" s="7"/>
-      <c r="BG61" s="7"/>
-    </row>
-    <row r="62" spans="1:59">
+      <c r="BH61" s="7"/>
+      <c r="BI61" s="7"/>
+    </row>
+    <row r="62" spans="1:61">
       <c r="A62" s="11">
         <v>106</v>
       </c>
@@ -8771,9 +8797,9 @@
       <c r="AI62" s="7">
         <v>0.18</v>
       </c>
-      <c r="BG62" s="11"/>
-    </row>
-    <row r="63" spans="1:59">
+      <c r="BI62" s="11"/>
+    </row>
+    <row r="63" spans="1:61">
       <c r="A63" s="11">
         <v>99</v>
       </c>
@@ -8852,20 +8878,26 @@
         <v>0.91</v>
       </c>
       <c r="AG63" s="1">
-        <v>0.24053630000000001</v>
+        <v>0.23280149999999999</v>
       </c>
       <c r="AH63" s="1">
-        <v>0.27668589999999998</v>
-      </c>
-      <c r="AI63" s="1">
-        <v>0.20249739999999999</v>
+        <v>0.27170080000000002</v>
+      </c>
+      <c r="AI63" s="26">
+        <v>0.19961490000000001</v>
       </c>
       <c r="AO63" s="1">
-        <v>1</v>
-      </c>
-      <c r="BG63" s="11"/>
-    </row>
-    <row r="64" spans="1:59">
+        <v>0.23280149999999999</v>
+      </c>
+      <c r="AP63" s="1">
+        <v>0.27170080000000002</v>
+      </c>
+      <c r="AQ63" s="26">
+        <v>0.19961490000000001</v>
+      </c>
+      <c r="BI63" s="11"/>
+    </row>
+    <row r="64" spans="1:61">
       <c r="A64" s="11">
         <v>94</v>
       </c>
@@ -8926,16 +8958,16 @@
       <c r="AE64" s="7">
         <v>0.66100000000000003</v>
       </c>
-      <c r="AP64" s="1" t="s">
+      <c r="AR64" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="BB64" s="1">
+      <c r="BD64" s="1">
         <v>1</v>
       </c>
-      <c r="BF64" s="7"/>
-      <c r="BG64" s="11"/>
-    </row>
-    <row r="65" spans="1:59">
+      <c r="BH64" s="7"/>
+      <c r="BI64" s="11"/>
+    </row>
+    <row r="65" spans="1:61">
       <c r="A65" s="11">
         <v>51</v>
       </c>
@@ -8958,15 +8990,15 @@
       <c r="V65" s="12"/>
       <c r="W65" s="12"/>
       <c r="X65" s="14"/>
-      <c r="AP65" s="1" t="s">
+      <c r="AR65" s="1" t="s">
         <v>1209</v>
       </c>
-      <c r="AZ65" s="1">
+      <c r="BB65" s="1">
         <v>1</v>
       </c>
-      <c r="BG65" s="11"/>
-    </row>
-    <row r="66" spans="1:59">
+      <c r="BI65" s="11"/>
+    </row>
+    <row r="66" spans="1:61">
       <c r="A66" s="11">
         <v>95</v>
       </c>
@@ -8989,16 +9021,16 @@
       <c r="V66" s="12"/>
       <c r="W66" s="12"/>
       <c r="X66" s="14"/>
-      <c r="AP66" s="1" t="s">
+      <c r="AR66" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="BC66" s="1">
+      <c r="BE66" s="1">
         <v>1</v>
       </c>
-      <c r="BF66" s="7"/>
-      <c r="BG66" s="11"/>
-    </row>
-    <row r="67" spans="1:59">
+      <c r="BH66" s="7"/>
+      <c r="BI66" s="11"/>
+    </row>
+    <row r="67" spans="1:61">
       <c r="A67" s="11">
         <v>85</v>
       </c>
@@ -9030,16 +9062,16 @@
       <c r="V67" s="12"/>
       <c r="W67" s="12"/>
       <c r="X67" s="14"/>
-      <c r="AP67" s="1" t="s">
+      <c r="AR67" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="BB67" s="1">
+      <c r="BD67" s="1">
         <v>1</v>
       </c>
-      <c r="BF67" s="7"/>
-      <c r="BG67" s="11"/>
-    </row>
-    <row r="68" spans="1:59">
+      <c r="BH67" s="7"/>
+      <c r="BI67" s="11"/>
+    </row>
+    <row r="68" spans="1:61">
       <c r="A68" s="11">
         <v>110</v>
       </c>
@@ -9058,16 +9090,16 @@
       <c r="F68" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="AP68" s="1" t="s">
+      <c r="AR68" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="BA68" s="1">
+      <c r="BC68" s="1">
         <v>1</v>
       </c>
-      <c r="BF68" s="7"/>
-      <c r="BG68" s="11"/>
-    </row>
-    <row r="69" spans="1:59">
+      <c r="BH68" s="7"/>
+      <c r="BI68" s="11"/>
+    </row>
+    <row r="69" spans="1:61">
       <c r="A69" s="11">
         <v>73</v>
       </c>
@@ -9131,9 +9163,9 @@
       <c r="AA69" s="9">
         <v>0.77400000000000002</v>
       </c>
-      <c r="BG69" s="11"/>
-    </row>
-    <row r="70" spans="1:59">
+      <c r="BI69" s="11"/>
+    </row>
+    <row r="70" spans="1:61">
       <c r="A70" s="7">
         <v>73</v>
       </c>
@@ -9191,15 +9223,15 @@
       <c r="AA70" s="9">
         <v>0.98399999999999999</v>
       </c>
-      <c r="AP70" s="1" t="s">
+      <c r="AR70" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="BA70" s="1">
+      <c r="BC70" s="1">
         <v>1</v>
       </c>
-      <c r="BG70" s="7"/>
-    </row>
-    <row r="71" spans="1:59">
+      <c r="BI70" s="7"/>
+    </row>
+    <row r="71" spans="1:61">
       <c r="A71" s="11">
         <v>80</v>
       </c>
@@ -9218,16 +9250,16 @@
       <c r="F71" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="AP71" s="1" t="s">
+      <c r="AR71" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="BC71" s="1">
+      <c r="BE71" s="1">
         <v>1</v>
       </c>
-      <c r="BF71" s="7"/>
-      <c r="BG71" s="11"/>
-    </row>
-    <row r="72" spans="1:59">
+      <c r="BH71" s="7"/>
+      <c r="BI71" s="11"/>
+    </row>
+    <row r="72" spans="1:61">
       <c r="A72" s="11">
         <v>52</v>
       </c>
@@ -9246,16 +9278,16 @@
       <c r="F72" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="AP72" s="1" t="s">
+      <c r="AR72" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="BB72" s="1">
+      <c r="BD72" s="1">
         <v>1</v>
       </c>
-      <c r="BF72" s="7"/>
-      <c r="BG72" s="11"/>
-    </row>
-    <row r="73" spans="1:59">
+      <c r="BH72" s="7"/>
+      <c r="BI72" s="11"/>
+    </row>
+    <row r="73" spans="1:61">
       <c r="A73" s="11">
         <v>83</v>
       </c>
@@ -9310,22 +9342,22 @@
       <c r="AJ73" s="9">
         <v>224</v>
       </c>
-      <c r="AP73" s="1" t="s">
+      <c r="AR73" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="AR73" s="1">
+      <c r="AT73" s="1">
         <v>34</v>
       </c>
-      <c r="AS73" s="1">
+      <c r="AU73" s="1">
         <v>42676</v>
       </c>
-      <c r="BD73" s="1">
+      <c r="BF73" s="1">
         <v>1</v>
       </c>
-      <c r="BF73" s="7"/>
-      <c r="BG73" s="11"/>
-    </row>
-    <row r="74" spans="1:59">
+      <c r="BH73" s="7"/>
+      <c r="BI73" s="11"/>
+    </row>
+    <row r="74" spans="1:61">
       <c r="A74" s="11">
         <v>91</v>
       </c>
@@ -9398,9 +9430,9 @@
       <c r="AI74" s="1">
         <v>0.189</v>
       </c>
-      <c r="BG74" s="11"/>
-    </row>
-    <row r="75" spans="1:59">
+      <c r="BI74" s="11"/>
+    </row>
+    <row r="75" spans="1:61">
       <c r="A75" s="11">
         <v>72</v>
       </c>
@@ -9503,21 +9535,21 @@
       <c r="AI75" s="7">
         <v>0.05</v>
       </c>
-      <c r="AV75" s="1">
+      <c r="AX75" s="1">
         <v>0.17</v>
       </c>
-      <c r="AW75" s="1">
+      <c r="AY75" s="1">
         <v>0.94399999999999995</v>
       </c>
-      <c r="AX75" s="1">
+      <c r="AZ75" s="1">
         <v>0.31</v>
       </c>
-      <c r="AY75" s="1">
+      <c r="BA75" s="1">
         <v>0.999</v>
       </c>
-      <c r="BG75" s="11"/>
-    </row>
-    <row r="76" spans="1:59">
+      <c r="BI75" s="11"/>
+    </row>
+    <row r="76" spans="1:61">
       <c r="A76" s="11">
         <v>92</v>
       </c>
@@ -9584,9 +9616,9 @@
       <c r="AF76" s="7">
         <v>0.89</v>
       </c>
-      <c r="BG76" s="11"/>
-    </row>
-    <row r="77" spans="1:59">
+      <c r="BI76" s="11"/>
+    </row>
+    <row r="77" spans="1:61">
       <c r="A77" s="11">
         <v>58</v>
       </c>
@@ -9605,16 +9637,16 @@
       <c r="F77" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="AP77" s="1" t="s">
+      <c r="AR77" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="BB77" s="1">
+      <c r="BD77" s="1">
         <v>1</v>
       </c>
-      <c r="BF77" s="7"/>
-      <c r="BG77" s="11"/>
-    </row>
-    <row r="78" spans="1:59">
+      <c r="BH77" s="7"/>
+      <c r="BI77" s="11"/>
+    </row>
+    <row r="78" spans="1:61">
       <c r="A78" s="11">
         <v>44</v>
       </c>
@@ -9717,9 +9749,9 @@
       <c r="AI78" s="7">
         <v>0.18</v>
       </c>
-      <c r="BG78" s="11"/>
-    </row>
-    <row r="79" spans="1:59">
+      <c r="BI78" s="11"/>
+    </row>
+    <row r="79" spans="1:61">
       <c r="A79" s="11">
         <v>55</v>
       </c>
@@ -9738,16 +9770,16 @@
       <c r="F79" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="AP79" s="1" t="s">
+      <c r="AR79" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="BA79" s="1">
+      <c r="BC79" s="1">
         <v>1</v>
       </c>
-      <c r="BF79" s="7"/>
-      <c r="BG79" s="11"/>
-    </row>
-    <row r="80" spans="1:59">
+      <c r="BH79" s="7"/>
+      <c r="BI79" s="11"/>
+    </row>
+    <row r="80" spans="1:61">
       <c r="A80" s="11">
         <v>43</v>
       </c>
@@ -9766,16 +9798,16 @@
       <c r="F80" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="AP80" s="1" t="s">
+      <c r="AR80" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="BB80" s="1">
+      <c r="BD80" s="1">
         <v>1</v>
       </c>
-      <c r="BF80" s="7"/>
-      <c r="BG80" s="11"/>
-    </row>
-    <row r="81" spans="1:59">
+      <c r="BH80" s="7"/>
+      <c r="BI80" s="11"/>
+    </row>
+    <row r="81" spans="1:61">
       <c r="A81" s="11">
         <v>40</v>
       </c>
@@ -9860,30 +9892,30 @@
       <c r="AI81" s="7">
         <v>0.19</v>
       </c>
-      <c r="AQ81" s="1" t="s">
+      <c r="AS81" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="AT81" s="1">
+      <c r="AV81" s="1">
         <v>0.02</v>
       </c>
-      <c r="AU81" s="1">
+      <c r="AW81" s="1">
         <v>0.93</v>
       </c>
-      <c r="AV81" s="1">
+      <c r="AX81" s="1">
         <v>0.12</v>
-      </c>
-      <c r="AW81" s="1">
-        <v>1</v>
-      </c>
-      <c r="AX81" s="1">
-        <v>0.24</v>
       </c>
       <c r="AY81" s="1">
         <v>1</v>
       </c>
-      <c r="BG81" s="11"/>
-    </row>
-    <row r="82" spans="1:59">
+      <c r="AZ81" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="BA81" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI81" s="11"/>
+    </row>
+    <row r="82" spans="1:61">
       <c r="A82" s="11">
         <v>81</v>
       </c>
@@ -9926,19 +9958,19 @@
       <c r="AM82" s="1">
         <v>153</v>
       </c>
-      <c r="AR82" s="1">
+      <c r="AT82" s="1">
         <v>25</v>
       </c>
-      <c r="AS82" s="1">
+      <c r="AU82" s="1">
         <v>1097</v>
       </c>
-      <c r="BD82" s="1">
+      <c r="BF82" s="1">
         <v>1</v>
       </c>
-      <c r="BF82" s="7"/>
-      <c r="BG82" s="11"/>
-    </row>
-    <row r="83" spans="1:59">
+      <c r="BH82" s="7"/>
+      <c r="BI82" s="11"/>
+    </row>
+    <row r="83" spans="1:61">
       <c r="A83" s="7">
         <v>81</v>
       </c>
@@ -9975,16 +10007,16 @@
       <c r="AM83" s="1">
         <v>5975</v>
       </c>
-      <c r="AR83" s="1">
+      <c r="AT83" s="1">
         <v>69</v>
       </c>
-      <c r="AS83" s="1">
+      <c r="AU83" s="1">
         <v>78041</v>
       </c>
-      <c r="BF83" s="7"/>
-      <c r="BG83" s="7"/>
-    </row>
-    <row r="84" spans="1:59">
+      <c r="BH83" s="7"/>
+      <c r="BI83" s="7"/>
+    </row>
+    <row r="84" spans="1:61">
       <c r="A84" s="11">
         <v>59</v>
       </c>
@@ -10052,7 +10084,7 @@
         <v>0.92</v>
       </c>
       <c r="AG84" s="26">
-        <v>0.2476749</v>
+        <v>0.24723990000000001</v>
       </c>
       <c r="AH84" s="26">
         <v>0.2476749</v>
@@ -10060,15 +10092,21 @@
       <c r="AI84" s="26">
         <v>0.1364398</v>
       </c>
-      <c r="AO84" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ84" s="1" t="s">
+      <c r="AO84" s="26">
+        <v>0.24723990000000001</v>
+      </c>
+      <c r="AP84" s="26">
+        <v>0.2476749</v>
+      </c>
+      <c r="AQ84" s="26">
+        <v>0.1364398</v>
+      </c>
+      <c r="AS84" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="BG84" s="11"/>
-    </row>
-    <row r="85" spans="1:59">
+      <c r="BI84" s="11"/>
+    </row>
+    <row r="85" spans="1:61">
       <c r="A85">
         <v>108</v>
       </c>
@@ -10114,15 +10152,15 @@
       <c r="S85" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="AP85" s="1" t="s">
+      <c r="AR85" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="BB85" s="1">
+      <c r="BD85" s="1">
         <v>1</v>
       </c>
-      <c r="BG85"/>
-    </row>
-    <row r="86" spans="1:59">
+      <c r="BI85"/>
+    </row>
+    <row r="86" spans="1:61">
       <c r="A86">
         <v>105</v>
       </c>
@@ -10141,15 +10179,15 @@
       <c r="F86" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="AP86" s="1" t="s">
+      <c r="AR86" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="AZ86" s="1">
+      <c r="BB86" s="1">
         <v>1</v>
       </c>
-      <c r="BG86"/>
-    </row>
-    <row r="87" spans="1:59">
+      <c r="BI86"/>
+    </row>
+    <row r="87" spans="1:61">
       <c r="A87">
         <v>62</v>
       </c>
@@ -10223,14 +10261,20 @@
         <v>0.27764349999999999</v>
       </c>
       <c r="AO87" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ87" s="1" t="s">
+        <v>0.2628393</v>
+      </c>
+      <c r="AP87" s="26">
+        <v>0.30556129999999998</v>
+      </c>
+      <c r="AQ87" s="26">
+        <v>0.27764349999999999</v>
+      </c>
+      <c r="AS87" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="BG87"/>
-    </row>
-    <row r="88" spans="1:59">
+      <c r="BI87"/>
+    </row>
+    <row r="88" spans="1:61">
       <c r="A88">
         <v>101</v>
       </c>
@@ -10249,15 +10293,15 @@
       <c r="F88" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="AP88" s="1" t="s">
+      <c r="AR88" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="AZ88" s="1">
+      <c r="BB88" s="1">
         <v>1</v>
       </c>
-      <c r="BG88"/>
-    </row>
-    <row r="89" spans="1:59">
+      <c r="BI88"/>
+    </row>
+    <row r="89" spans="1:61">
       <c r="A89">
         <v>76</v>
       </c>
@@ -10315,21 +10359,21 @@
       <c r="AM89" s="1">
         <v>23</v>
       </c>
-      <c r="AP89" s="1" t="s">
+      <c r="AR89" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="AR89" s="1">
+      <c r="AT89" s="1">
         <v>6</v>
       </c>
-      <c r="AS89" s="1">
+      <c r="AU89" s="1">
         <v>80</v>
       </c>
-      <c r="BD89" s="1">
+      <c r="BF89" s="1">
         <v>1</v>
       </c>
-      <c r="BG89"/>
-    </row>
-    <row r="90" spans="1:59">
+      <c r="BI89"/>
+    </row>
+    <row r="90" spans="1:61">
       <c r="A90">
         <v>76</v>
       </c>
@@ -10384,18 +10428,18 @@
       <c r="AM90" s="1">
         <v>32</v>
       </c>
-      <c r="AP90" s="1" t="s">
+      <c r="AR90" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="AR90" s="1">
+      <c r="AT90" s="1">
         <v>9</v>
       </c>
-      <c r="AS90" s="1">
+      <c r="AU90" s="1">
         <v>132</v>
       </c>
-      <c r="BG90"/>
-    </row>
-    <row r="91" spans="1:59">
+      <c r="BI90"/>
+    </row>
+    <row r="91" spans="1:61">
       <c r="A91">
         <v>76</v>
       </c>
@@ -10450,18 +10494,18 @@
       <c r="AM91" s="1">
         <v>117</v>
       </c>
-      <c r="AP91" s="1" t="s">
+      <c r="AR91" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="AR91" s="1">
+      <c r="AT91" s="1">
         <v>7</v>
       </c>
-      <c r="AS91" s="1">
+      <c r="AU91" s="1">
         <v>278</v>
       </c>
-      <c r="BG91"/>
-    </row>
-    <row r="92" spans="1:59">
+      <c r="BI91"/>
+    </row>
+    <row r="92" spans="1:61">
       <c r="A92">
         <v>76</v>
       </c>
@@ -10516,18 +10560,18 @@
       <c r="AM92" s="1">
         <v>92</v>
       </c>
-      <c r="AP92" s="1" t="s">
+      <c r="AR92" s="1" t="s">
         <v>1129</v>
       </c>
-      <c r="AR92" s="1">
+      <c r="AT92" s="1">
         <v>14</v>
       </c>
-      <c r="AS92" s="1">
+      <c r="AU92" s="1">
         <v>55</v>
       </c>
-      <c r="BG92"/>
-    </row>
-    <row r="93" spans="1:59">
+      <c r="BI92"/>
+    </row>
+    <row r="93" spans="1:61">
       <c r="A93">
         <v>76</v>
       </c>
@@ -10579,18 +10623,18 @@
       <c r="AM93" s="1">
         <v>78</v>
       </c>
-      <c r="AP93" s="1" t="s">
+      <c r="AR93" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="AR93" s="1">
+      <c r="AT93" s="1">
         <v>1</v>
       </c>
-      <c r="AS93" s="1">
+      <c r="AU93" s="1">
         <v>74</v>
       </c>
-      <c r="BG93"/>
-    </row>
-    <row r="94" spans="1:59">
+      <c r="BI93"/>
+    </row>
+    <row r="94" spans="1:61">
       <c r="A94">
         <v>76</v>
       </c>
@@ -10645,18 +10689,18 @@
       <c r="AM94" s="1">
         <v>108</v>
       </c>
-      <c r="AP94" s="1" t="s">
+      <c r="AR94" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="AR94" s="1">
+      <c r="AT94" s="1">
         <v>7</v>
       </c>
-      <c r="AS94" s="1">
+      <c r="AU94" s="1">
         <v>128</v>
       </c>
-      <c r="BG94"/>
-    </row>
-    <row r="95" spans="1:59">
+      <c r="BI94"/>
+    </row>
+    <row r="95" spans="1:61">
       <c r="A95">
         <v>76</v>
       </c>
@@ -10711,18 +10755,18 @@
       <c r="AM95" s="1">
         <v>72</v>
       </c>
-      <c r="AP95" s="1" t="s">
+      <c r="AR95" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="AR95" s="1">
+      <c r="AT95" s="1">
         <v>12</v>
       </c>
-      <c r="AS95" s="1">
+      <c r="AU95" s="1">
         <v>887</v>
       </c>
-      <c r="BG95"/>
-    </row>
-    <row r="96" spans="1:59">
+      <c r="BI95"/>
+    </row>
+    <row r="96" spans="1:61">
       <c r="A96">
         <v>42</v>
       </c>
@@ -10807,15 +10851,21 @@
       <c r="AM96" s="1">
         <v>199.7</v>
       </c>
-      <c r="AO96" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ96" s="1" t="s">
+      <c r="AO96" s="26">
+        <v>0.1958955</v>
+      </c>
+      <c r="AP96" s="26">
+        <v>0.25844519999999999</v>
+      </c>
+      <c r="AQ96" s="26">
+        <v>0.16113340000000001</v>
+      </c>
+      <c r="AS96" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="BG96"/>
-    </row>
-    <row r="97" spans="1:59">
+      <c r="BI96"/>
+    </row>
+    <row r="97" spans="1:61">
       <c r="A97">
         <v>89</v>
       </c>
@@ -10882,9 +10932,9 @@
       <c r="AF97" s="7">
         <v>0.98</v>
       </c>
-      <c r="BG97"/>
-    </row>
-    <row r="98" spans="1:59">
+      <c r="BI97"/>
+    </row>
+    <row r="98" spans="1:61">
       <c r="A98">
         <v>50</v>
       </c>
@@ -10987,30 +11037,30 @@
       <c r="AI98" s="7">
         <v>0.184</v>
       </c>
-      <c r="AQ98" s="1" t="s">
+      <c r="AS98" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="AT98" s="1">
+      <c r="AV98" s="1">
         <v>0.93</v>
       </c>
-      <c r="AU98" s="1">
+      <c r="AW98" s="1">
         <v>0.19800000000000001</v>
       </c>
-      <c r="AV98" s="1">
+      <c r="AX98" s="1">
         <v>0.36499999999999999</v>
       </c>
-      <c r="AW98" s="1">
+      <c r="AY98" s="1">
         <v>0.45900000000000002</v>
       </c>
-      <c r="AX98" s="1">
+      <c r="AZ98" s="1">
         <v>0.76</v>
       </c>
-      <c r="AY98" s="1">
+      <c r="BA98" s="1">
         <v>0.95</v>
       </c>
-      <c r="BG98"/>
-    </row>
-    <row r="99" spans="1:59">
+      <c r="BI98"/>
+    </row>
+    <row r="99" spans="1:61">
       <c r="A99" s="1">
         <v>50</v>
       </c>
@@ -11107,26 +11157,26 @@
       <c r="AI99" s="7">
         <v>0.223</v>
       </c>
-      <c r="AT99" s="1">
+      <c r="AV99" s="1">
         <v>0.06</v>
       </c>
-      <c r="AU99" s="1">
+      <c r="AW99" s="1">
         <v>0.15</v>
       </c>
-      <c r="AV99" s="1">
+      <c r="AX99" s="1">
         <v>0.32</v>
       </c>
-      <c r="AW99" s="1">
+      <c r="AY99" s="1">
         <v>0.36899999999999999</v>
       </c>
-      <c r="AX99" s="1">
+      <c r="AZ99" s="1">
         <v>0.99</v>
       </c>
-      <c r="AY99" s="1">
+      <c r="BA99" s="1">
         <v>0.99</v>
       </c>
     </row>
-    <row r="100" spans="1:59">
+    <row r="100" spans="1:61">
       <c r="A100">
         <v>112</v>
       </c>
@@ -11181,6 +11231,15 @@
       <c r="T100" s="1" t="s">
         <v>418</v>
       </c>
+      <c r="AD100" s="7">
+        <v>0.27</v>
+      </c>
+      <c r="AE100" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="AF100" s="7">
+        <v>0.89</v>
+      </c>
       <c r="AG100" s="7">
         <v>0.17</v>
       </c>
@@ -11190,9 +11249,9 @@
       <c r="AI100" s="7">
         <v>0.19</v>
       </c>
-      <c r="BG100"/>
-    </row>
-    <row r="101" spans="1:59">
+      <c r="BI100"/>
+    </row>
+    <row r="101" spans="1:61">
       <c r="A101" s="1">
         <v>112</v>
       </c>
@@ -11238,6 +11297,15 @@
       <c r="T101" s="1" t="s">
         <v>418</v>
       </c>
+      <c r="AD101" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AE101" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AF101" s="7">
+        <v>0.84</v>
+      </c>
       <c r="AG101" s="7">
         <v>0.27</v>
       </c>
@@ -11248,7 +11316,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="102" spans="1:59">
+    <row r="102" spans="1:61">
       <c r="A102">
         <v>70</v>
       </c>
@@ -11300,21 +11368,21 @@
       <c r="AN102" s="1">
         <v>12.09</v>
       </c>
-      <c r="AP102" s="1" t="s">
+      <c r="AR102" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="AR102" s="1">
+      <c r="AT102" s="1">
         <v>5</v>
       </c>
-      <c r="AS102" s="1">
+      <c r="AU102" s="1">
         <v>114</v>
       </c>
-      <c r="BB102" s="1">
+      <c r="BD102" s="1">
         <v>1</v>
       </c>
-      <c r="BG102"/>
-    </row>
-    <row r="103" spans="1:59">
+      <c r="BI102"/>
+    </row>
+    <row r="103" spans="1:61">
       <c r="A103">
         <v>47</v>
       </c>
@@ -11333,12 +11401,12 @@
       <c r="F103" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="BA103" s="1">
+      <c r="BC103" s="1">
         <v>1</v>
       </c>
-      <c r="BG103"/>
-    </row>
-    <row r="104" spans="1:59">
+      <c r="BI103"/>
+    </row>
+    <row r="104" spans="1:61">
       <c r="A104">
         <v>103</v>
       </c>
@@ -11447,12 +11515,12 @@
       <c r="AN104" s="1">
         <v>55</v>
       </c>
-      <c r="AQ104" s="1" t="s">
+      <c r="AS104" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="BG104"/>
-    </row>
-    <row r="105" spans="1:59">
+      <c r="BI104"/>
+    </row>
+    <row r="105" spans="1:61">
       <c r="A105">
         <v>97</v>
       </c>
@@ -11537,12 +11605,12 @@
       <c r="AI105" s="7">
         <v>0.13</v>
       </c>
-      <c r="AQ105" s="1" t="s">
+      <c r="AS105" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="BG105"/>
-    </row>
-    <row r="106" spans="1:59">
+      <c r="BI105"/>
+    </row>
+    <row r="106" spans="1:61">
       <c r="A106">
         <v>65</v>
       </c>
@@ -11661,33 +11729,35 @@
         <v>35.090000000000003</v>
       </c>
       <c r="AO106" s="7"/>
-      <c r="AR106" s="1">
+      <c r="AP106" s="7"/>
+      <c r="AQ106" s="7"/>
+      <c r="AT106" s="1">
         <v>15</v>
       </c>
-      <c r="AS106" s="1">
+      <c r="AU106" s="1">
         <v>150</v>
       </c>
-      <c r="AT106" s="1">
+      <c r="AV106" s="1">
         <v>0.06</v>
       </c>
-      <c r="AU106" s="1">
+      <c r="AW106" s="1">
         <v>0.23</v>
       </c>
-      <c r="AV106" s="1">
+      <c r="AX106" s="1">
         <v>0.11</v>
       </c>
-      <c r="AW106" s="1">
+      <c r="AY106" s="1">
         <v>0.86</v>
       </c>
-      <c r="AX106" s="1">
+      <c r="AZ106" s="1">
         <v>0.22</v>
       </c>
-      <c r="AY106" s="1">
+      <c r="BA106" s="1">
         <v>0.99</v>
       </c>
-      <c r="BG106"/>
-    </row>
-    <row r="107" spans="1:59">
+      <c r="BI106"/>
+    </row>
+    <row r="107" spans="1:61">
       <c r="A107" s="11">
         <v>113</v>
       </c>
@@ -11755,12 +11825,12 @@
         <v>0.78</v>
       </c>
       <c r="AG107" s="7"/>
-      <c r="AQ107" s="1" t="s">
+      <c r="AS107" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="BG107" s="11"/>
-    </row>
-    <row r="108" spans="1:59">
+      <c r="BI107" s="11"/>
+    </row>
+    <row r="108" spans="1:61">
       <c r="A108" s="11">
         <v>118</v>
       </c>
@@ -11842,9 +11912,9 @@
       <c r="AI108" s="7">
         <v>0.1</v>
       </c>
-      <c r="BG108" s="11"/>
-    </row>
-    <row r="109" spans="1:59">
+      <c r="BI108" s="11"/>
+    </row>
+    <row r="109" spans="1:61">
       <c r="A109" s="11">
         <v>118</v>
       </c>
@@ -11917,12 +11987,12 @@
       <c r="AI109" s="7">
         <v>0.02</v>
       </c>
-      <c r="AQ109" s="1" t="s">
+      <c r="AS109" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="BG109" s="7"/>
-    </row>
-    <row r="110" spans="1:59">
+      <c r="BI109" s="7"/>
+    </row>
+    <row r="110" spans="1:61">
       <c r="A110" s="11">
         <v>121</v>
       </c>
@@ -11995,18 +12065,24 @@
       <c r="AI110" s="7">
         <v>0.2384077</v>
       </c>
-      <c r="AO110" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP110" s="1" t="s">
+      <c r="AO110" s="26">
+        <v>0.21827099999999999</v>
+      </c>
+      <c r="AP110" s="26">
+        <v>0.2890624</v>
+      </c>
+      <c r="AQ110" s="7">
+        <v>0.2384077</v>
+      </c>
+      <c r="AR110" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="AQ110" s="1" t="s">
+      <c r="AS110" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="BG110" s="11"/>
-    </row>
-    <row r="111" spans="1:59">
+      <c r="BI110" s="11"/>
+    </row>
+    <row r="111" spans="1:61">
       <c r="A111" s="11">
         <v>115</v>
       </c>
@@ -12079,15 +12155,15 @@
       <c r="AI111" s="7">
         <v>0.2482</v>
       </c>
-      <c r="AP111" s="1" t="s">
-        <v>1214</v>
-      </c>
-      <c r="AQ111" s="1" t="s">
+      <c r="AR111" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="AS111" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="BG111" s="11"/>
-    </row>
-    <row r="112" spans="1:59">
+      <c r="BI111" s="11"/>
+    </row>
+    <row r="112" spans="1:61">
       <c r="A112" s="11">
         <v>117</v>
       </c>
@@ -12181,12 +12257,12 @@
       <c r="AF112" s="7">
         <v>0.73</v>
       </c>
-      <c r="AQ112" s="1" t="s">
+      <c r="AS112" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="BG112" s="11"/>
-    </row>
-    <row r="113" spans="1:59">
+      <c r="BI112" s="11"/>
+    </row>
+    <row r="113" spans="1:61">
       <c r="A113" s="11">
         <v>116</v>
       </c>
@@ -12289,12 +12365,12 @@
       <c r="AI113" s="7">
         <v>0.21</v>
       </c>
-      <c r="AQ113" s="1" t="s">
+      <c r="AS113" s="1" t="s">
         <v>873</v>
       </c>
-      <c r="BG113" s="11"/>
-    </row>
-    <row r="114" spans="1:59">
+      <c r="BI113" s="11"/>
+    </row>
+    <row r="114" spans="1:61">
       <c r="A114" s="11">
         <v>123</v>
       </c>
@@ -12370,12 +12446,12 @@
       <c r="AF114" s="7">
         <v>0.71</v>
       </c>
-      <c r="AQ114" s="1" t="s">
+      <c r="AS114" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="BG114" s="11"/>
-    </row>
-    <row r="115" spans="1:59">
+      <c r="BI114" s="11"/>
+    </row>
+    <row r="115" spans="1:61">
       <c r="A115" s="11">
         <v>119</v>
       </c>
@@ -12452,7 +12528,7 @@
         <v>0.83</v>
       </c>
       <c r="AG115" s="7">
-        <v>0.23168449999999999</v>
+        <v>0.23280149999999999</v>
       </c>
       <c r="AH115" s="7">
         <v>0.27170080000000002</v>
@@ -12460,15 +12536,21 @@
       <c r="AI115" s="7">
         <v>0.19961490000000001</v>
       </c>
-      <c r="AO115" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ115" s="1" t="s">
+      <c r="AO115" s="7">
+        <v>0.23280149999999999</v>
+      </c>
+      <c r="AP115" s="7">
+        <v>0.27170080000000002</v>
+      </c>
+      <c r="AQ115" s="7">
+        <v>0.19961490000000001</v>
+      </c>
+      <c r="AS115" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="BG115" s="11"/>
-    </row>
-    <row r="116" spans="1:59">
+      <c r="BI115" s="11"/>
+    </row>
+    <row r="116" spans="1:61">
       <c r="A116" s="11">
         <v>114</v>
       </c>
@@ -12545,12 +12627,12 @@
       <c r="AI116" s="7">
         <v>0.04</v>
       </c>
-      <c r="AQ116" s="1" t="s">
+      <c r="AS116" s="1" t="s">
         <v>888</v>
       </c>
-      <c r="BG116" s="11"/>
-    </row>
-    <row r="117" spans="1:59">
+      <c r="BI116" s="11"/>
+    </row>
+    <row r="117" spans="1:61">
       <c r="A117" s="11">
         <v>114</v>
       </c>
@@ -12621,9 +12703,9 @@
       <c r="AI117" s="7">
         <v>0.9</v>
       </c>
-      <c r="BG117" s="11"/>
-    </row>
-    <row r="118" spans="1:59">
+      <c r="BI117" s="11"/>
+    </row>
+    <row r="118" spans="1:61">
       <c r="A118" s="11">
         <v>114</v>
       </c>
@@ -12694,9 +12776,9 @@
       <c r="AI118" s="7">
         <v>0.05</v>
       </c>
-      <c r="BG118" s="11"/>
-    </row>
-    <row r="119" spans="1:59">
+      <c r="BI118" s="11"/>
+    </row>
+    <row r="119" spans="1:61">
       <c r="A119" s="7">
         <v>114</v>
       </c>
@@ -12767,9 +12849,9 @@
       <c r="AI119" s="7">
         <v>0.11</v>
       </c>
-      <c r="BG119" s="7"/>
-    </row>
-    <row r="120" spans="1:59">
+      <c r="BI119" s="7"/>
+    </row>
+    <row r="120" spans="1:61">
       <c r="A120" s="11">
         <v>122</v>
       </c>
@@ -12813,7 +12895,7 @@
         <v>66</v>
       </c>
       <c r="P120" s="1">
-        <v>7</v>
+        <v>867</v>
       </c>
       <c r="Q120" s="1" t="s">
         <v>674</v>
@@ -12836,12 +12918,12 @@
       <c r="AF120" s="7">
         <v>0.87</v>
       </c>
-      <c r="AQ120" s="1" t="s">
+      <c r="AS120" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="BG120" s="11"/>
-    </row>
-    <row r="121" spans="1:59">
+      <c r="BI120" s="11"/>
+    </row>
+    <row r="121" spans="1:61">
       <c r="A121" s="11">
         <v>120</v>
       </c>
@@ -12878,16 +12960,16 @@
       <c r="L121" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="AP121" s="1" t="s">
+      <c r="AR121" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="BB121" s="1">
+      <c r="BD121" s="1">
         <v>1</v>
       </c>
-      <c r="BF121" s="7"/>
-      <c r="BG121" s="11"/>
-    </row>
-    <row r="122" spans="1:59">
+      <c r="BH121" s="7"/>
+      <c r="BI121" s="11"/>
+    </row>
+    <row r="122" spans="1:61">
       <c r="A122">
         <v>129</v>
       </c>
@@ -12969,12 +13051,12 @@
       <c r="AI122" s="7">
         <v>0.19</v>
       </c>
-      <c r="AQ122" s="1" t="s">
+      <c r="AS122" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="BG122"/>
-    </row>
-    <row r="123" spans="1:59">
+      <c r="BI122"/>
+    </row>
+    <row r="123" spans="1:61">
       <c r="A123">
         <v>126</v>
       </c>
@@ -13074,12 +13156,12 @@
       <c r="AI123" s="7">
         <v>0.2830194339616981</v>
       </c>
-      <c r="AQ123" s="1" t="s">
+      <c r="AS123" s="1" t="s">
         <v>1004</v>
       </c>
-      <c r="BG123"/>
-    </row>
-    <row r="124" spans="1:59">
+      <c r="BI123"/>
+    </row>
+    <row r="124" spans="1:61">
       <c r="A124">
         <v>124</v>
       </c>
@@ -13164,15 +13246,21 @@
       <c r="AI124" s="7">
         <v>0.13164390000000001</v>
       </c>
-      <c r="AO124" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ124" s="1" t="s">
+      <c r="AO124" s="7">
+        <v>0.146394</v>
+      </c>
+      <c r="AP124" s="26">
+        <v>0.2219286</v>
+      </c>
+      <c r="AQ124" s="7">
+        <v>0.13164390000000001</v>
+      </c>
+      <c r="AS124" s="1" t="s">
         <v>1011</v>
       </c>
-      <c r="BG124"/>
-    </row>
-    <row r="125" spans="1:59">
+      <c r="BI124"/>
+    </row>
+    <row r="125" spans="1:61">
       <c r="A125">
         <v>131</v>
       </c>
@@ -13240,23 +13328,29 @@
         <v>0.85</v>
       </c>
       <c r="AG125" s="7">
-        <v>0.2081991</v>
+        <v>0.21291959999999999</v>
       </c>
       <c r="AH125" s="26">
-        <v>0.27312740000000002</v>
+        <v>0.27367229999999998</v>
       </c>
       <c r="AI125" s="26">
         <v>0.1919208</v>
       </c>
-      <c r="AO125" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ125" s="1" t="s">
+      <c r="AO125" s="7">
+        <v>0.21291959999999999</v>
+      </c>
+      <c r="AP125" s="26">
+        <v>0.27367229999999998</v>
+      </c>
+      <c r="AQ125" s="26">
+        <v>0.1919208</v>
+      </c>
+      <c r="AS125" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="BG125"/>
-    </row>
-    <row r="126" spans="1:59">
+      <c r="BI125"/>
+    </row>
+    <row r="126" spans="1:61">
       <c r="A126">
         <v>125</v>
       </c>
@@ -13341,12 +13435,12 @@
       <c r="AI126" s="7">
         <v>0.16</v>
       </c>
-      <c r="AQ126" s="1" t="s">
+      <c r="AS126" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="BG126"/>
-    </row>
-    <row r="127" spans="1:59">
+      <c r="BI126"/>
+    </row>
+    <row r="127" spans="1:61">
       <c r="A127">
         <v>127</v>
       </c>
@@ -13428,12 +13522,12 @@
       <c r="AI127" s="7">
         <v>0.16500000000000001</v>
       </c>
-      <c r="AQ127" s="1" t="s">
+      <c r="AS127" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="BG127"/>
-    </row>
-    <row r="128" spans="1:59">
+      <c r="BI127"/>
+    </row>
+    <row r="128" spans="1:61">
       <c r="A128">
         <v>129</v>
       </c>
@@ -13461,13 +13555,13 @@
       <c r="O128" s="1">
         <v>697</v>
       </c>
-      <c r="AP128" s="1" t="s">
+      <c r="AR128" s="1" t="s">
         <v>1029</v>
       </c>
-      <c r="BE128" s="1">
+      <c r="BG128" s="1">
         <v>1</v>
       </c>
-      <c r="BG128"/>
+      <c r="BI128"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding in missing data imputation
</commit_message>
<xml_diff>
--- a/PowerEstimationReviewDataCollection2018.03.25.xlsx
+++ b/PowerEstimationReviewDataCollection2018.03.25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Systematic Reviews\History of Power Estimation Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C0F6D8-B6E9-4AD0-877F-BD1819DC3FCD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4618AFE5-8902-4702-8F9F-70F100E443AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="10640" windowHeight="5720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="1217">
   <si>
     <t>Author</t>
   </si>
@@ -4244,9 +4244,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="31" zoomScaleNormal="47" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="31" zoomScaleNormal="47" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI115" sqref="AI115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -9115,6 +9115,9 @@
       <c r="E69" s="11">
         <v>2015</v>
       </c>
+      <c r="F69" s="7" t="s">
+        <v>430</v>
+      </c>
       <c r="G69" s="1" t="s">
         <v>648</v>
       </c>
@@ -9162,6 +9165,9 @@
       </c>
       <c r="AA69" s="9">
         <v>0.77400000000000002</v>
+      </c>
+      <c r="AR69" s="1" t="s">
+        <v>602</v>
       </c>
       <c r="BI69" s="11"/>
     </row>
@@ -9174,6 +9180,9 @@
       </c>
       <c r="E70" s="11">
         <v>2015</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>430</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>648</v>

</xml_diff>

<commit_message>
Playing around with fitting distributions for mean estiamtion purposes
</commit_message>
<xml_diff>
--- a/PowerEstimationReviewDataCollection2018.03.25.xlsx
+++ b/PowerEstimationReviewDataCollection2018.03.25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Systematic Reviews\History of Power Estimation Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4618AFE5-8902-4702-8F9F-70F100E443AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6C8140-E504-44AB-9DC3-240A93C6942B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="10640" windowHeight="5720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <definedName name="_Hlk504467761" localSheetId="7">'Search terms'!$A$1</definedName>
     <definedName name="PowerEstimationStudiesLib_for_export" localSheetId="4">Randomisation_original_sample!$A$2:$I$75</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -3771,7 +3771,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4244,30 +4244,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="31" zoomScaleNormal="47" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI115" sqref="AI115"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="39" zoomScaleNormal="47" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="47.7890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.2890625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.9140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.9140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="32.20703125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="32.1640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="5.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.20703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.70703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7890625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7890625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.95703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.75" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.9140625" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.75" style="1" customWidth="1"/>
     <col min="21" max="21" width="14.9140625" style="9" customWidth="1"/>
     <col min="22" max="23" width="10.83203125" style="7" customWidth="1"/>
@@ -4285,7 +4285,7 @@
     <col min="61" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>414</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>100</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>49</v>
       </c>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="AV3" s="4"/>
     </row>
-    <row r="4" spans="1:61">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>49</v>
       </c>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="AV4" s="4"/>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>60</v>
       </c>
@@ -4756,7 +4756,7 @@
       <c r="AV5" s="4"/>
       <c r="BI5" s="7"/>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>77</v>
       </c>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="AV6" s="4"/>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>77</v>
       </c>
@@ -4940,7 +4940,7 @@
       <c r="AR7" s="4"/>
       <c r="AV7" s="4"/>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -5025,7 +5025,7 @@
       <c r="AR8" s="4"/>
       <c r="AV8" s="4"/>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>77</v>
       </c>
@@ -5110,7 +5110,7 @@
       <c r="AR9" s="4"/>
       <c r="AV9" s="4"/>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>77</v>
       </c>
@@ -5195,7 +5195,7 @@
       <c r="AR10" s="4"/>
       <c r="AV10" s="4"/>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>69</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>69</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>69</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>109</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>46</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>84</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:61">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>63</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:61">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>74</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:61">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>107</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:61">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>71</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="21" spans="1:61">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>113</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:61">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>66</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="23" spans="1:61">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>53</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:61">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>75</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="1:61">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>54</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:61">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>102</v>
       </c>
@@ -6389,7 +6389,7 @@
       </c>
       <c r="BI26" s="11"/>
     </row>
-    <row r="27" spans="1:61">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>90</v>
       </c>
@@ -6429,7 +6429,7 @@
       <c r="BH27" s="7"/>
       <c r="BI27" s="11"/>
     </row>
-    <row r="28" spans="1:61">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>61</v>
       </c>
@@ -6472,7 +6472,7 @@
       <c r="BH28" s="7"/>
       <c r="BI28" s="11"/>
     </row>
-    <row r="29" spans="1:61">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>86</v>
       </c>
@@ -6559,7 +6559,7 @@
       </c>
       <c r="BI29" s="11"/>
     </row>
-    <row r="30" spans="1:61">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>57</v>
       </c>
@@ -6635,7 +6635,7 @@
       <c r="BH30" s="7"/>
       <c r="BI30" s="11"/>
     </row>
-    <row r="31" spans="1:61">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>57</v>
       </c>
@@ -6702,7 +6702,7 @@
       <c r="BH31" s="7"/>
       <c r="BI31" s="11"/>
     </row>
-    <row r="32" spans="1:61">
+    <row r="32" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -6770,7 +6770,7 @@
       <c r="BH32" s="7"/>
       <c r="BI32" s="11"/>
     </row>
-    <row r="33" spans="1:61">
+    <row r="33" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>57</v>
       </c>
@@ -6838,7 +6838,7 @@
       <c r="BH33" s="7"/>
       <c r="BI33" s="11"/>
     </row>
-    <row r="34" spans="1:61">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>57</v>
       </c>
@@ -6906,7 +6906,7 @@
       <c r="BH34" s="7"/>
       <c r="BI34" s="11"/>
     </row>
-    <row r="35" spans="1:61">
+    <row r="35" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>57</v>
       </c>
@@ -6974,7 +6974,7 @@
       <c r="BH35" s="7"/>
       <c r="BI35" s="11"/>
     </row>
-    <row r="36" spans="1:61">
+    <row r="36" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>78</v>
       </c>
@@ -7054,7 +7054,7 @@
       <c r="BH36" s="7"/>
       <c r="BI36" s="11"/>
     </row>
-    <row r="37" spans="1:61">
+    <row r="37" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>64</v>
       </c>
@@ -7121,7 +7121,7 @@
       <c r="BH37" s="7"/>
       <c r="BI37" s="11"/>
     </row>
-    <row r="38" spans="1:61">
+    <row r="38" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>68</v>
       </c>
@@ -7241,7 +7241,7 @@
       </c>
       <c r="BI38" s="11"/>
     </row>
-    <row r="39" spans="1:61">
+    <row r="39" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>93</v>
       </c>
@@ -7311,7 +7311,7 @@
       <c r="BH39" s="7"/>
       <c r="BI39" s="11"/>
     </row>
-    <row r="40" spans="1:61">
+    <row r="40" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>48</v>
       </c>
@@ -7378,7 +7378,7 @@
       <c r="BH40" s="7"/>
       <c r="BI40" s="11"/>
     </row>
-    <row r="41" spans="1:61">
+    <row r="41" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A41" s="11">
         <v>48</v>
       </c>
@@ -7424,7 +7424,7 @@
       <c r="BH41" s="7"/>
       <c r="BI41" s="11"/>
     </row>
-    <row r="42" spans="1:61" s="11" customFormat="1">
+    <row r="42" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>88</v>
       </c>
@@ -7526,7 +7526,7 @@
       </c>
       <c r="AJ42" s="14"/>
     </row>
-    <row r="43" spans="1:61" s="11" customFormat="1">
+    <row r="43" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11">
         <v>111</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:61" s="11" customFormat="1">
+    <row r="44" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>111</v>
       </c>
@@ -7644,7 +7644,7 @@
       <c r="AP44" s="12"/>
       <c r="AQ44" s="12"/>
     </row>
-    <row r="45" spans="1:61" s="11" customFormat="1">
+    <row r="45" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>111</v>
       </c>
@@ -7697,7 +7697,7 @@
       <c r="AP45" s="13"/>
       <c r="AQ45" s="13"/>
     </row>
-    <row r="46" spans="1:61" s="11" customFormat="1">
+    <row r="46" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>111</v>
       </c>
@@ -7750,7 +7750,7 @@
       <c r="AP46" s="12"/>
       <c r="AQ46" s="12"/>
     </row>
-    <row r="47" spans="1:61" s="11" customFormat="1">
+    <row r="47" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
         <v>111</v>
       </c>
@@ -7803,7 +7803,7 @@
       <c r="AP47" s="12"/>
       <c r="AQ47" s="12"/>
     </row>
-    <row r="48" spans="1:61" s="11" customFormat="1">
+    <row r="48" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>56</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:61" s="11" customFormat="1">
+    <row r="49" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
         <v>82</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:61" s="11" customFormat="1">
+    <row r="50" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
         <v>104</v>
       </c>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="AJ50" s="14"/>
     </row>
-    <row r="51" spans="1:61" s="11" customFormat="1">
+    <row r="51" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
         <v>87</v>
       </c>
@@ -7980,7 +7980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:61" s="11" customFormat="1">
+    <row r="52" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="53" spans="1:61" s="11" customFormat="1">
+    <row r="53" spans="1:61" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
         <v>67</v>
       </c>
@@ -8190,7 +8190,7 @@
       <c r="AS53" s="1"/>
       <c r="AT53" s="1"/>
     </row>
-    <row r="54" spans="1:61">
+    <row r="54" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
         <v>96</v>
       </c>
@@ -8257,9 +8257,7 @@
       <c r="AE54" s="9">
         <v>0.81</v>
       </c>
-      <c r="AG54" s="26">
-        <v>0.3251309</v>
-      </c>
+      <c r="AG54" s="26"/>
       <c r="AO54" s="26">
         <v>0.3251309</v>
       </c>
@@ -8268,7 +8266,7 @@
       </c>
       <c r="BI54" s="11"/>
     </row>
-    <row r="55" spans="1:61">
+    <row r="55" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
         <v>98</v>
       </c>
@@ -8346,7 +8344,7 @@
       </c>
       <c r="BI55" s="11"/>
     </row>
-    <row r="56" spans="1:61">
+    <row r="56" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>79</v>
       </c>
@@ -8413,7 +8411,7 @@
       <c r="BH56" s="7"/>
       <c r="BI56" s="11"/>
     </row>
-    <row r="57" spans="1:61">
+    <row r="57" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
         <v>79</v>
       </c>
@@ -8471,7 +8469,7 @@
       <c r="BH57" s="7"/>
       <c r="BI57" s="11"/>
     </row>
-    <row r="58" spans="1:61">
+    <row r="58" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A58" s="11">
         <v>79</v>
       </c>
@@ -8529,7 +8527,7 @@
       <c r="BH58" s="7"/>
       <c r="BI58" s="11"/>
     </row>
-    <row r="59" spans="1:61">
+    <row r="59" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A59" s="11">
         <v>79</v>
       </c>
@@ -8587,7 +8585,7 @@
       <c r="BH59" s="7"/>
       <c r="BI59" s="11"/>
     </row>
-    <row r="60" spans="1:61">
+    <row r="60" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A60" s="11">
         <v>41</v>
       </c>
@@ -8645,7 +8643,7 @@
       <c r="BH60" s="7"/>
       <c r="BI60" s="11"/>
     </row>
-    <row r="61" spans="1:61">
+    <row r="61" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A61" s="7">
         <v>41</v>
       </c>
@@ -8694,7 +8692,7 @@
       <c r="BH61" s="7"/>
       <c r="BI61" s="7"/>
     </row>
-    <row r="62" spans="1:61">
+    <row r="62" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
         <v>106</v>
       </c>
@@ -8799,7 +8797,7 @@
       </c>
       <c r="BI62" s="11"/>
     </row>
-    <row r="63" spans="1:61">
+    <row r="63" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A63" s="11">
         <v>99</v>
       </c>
@@ -8877,15 +8875,7 @@
       <c r="AF63" s="7">
         <v>0.91</v>
       </c>
-      <c r="AG63" s="1">
-        <v>0.23280149999999999</v>
-      </c>
-      <c r="AH63" s="1">
-        <v>0.27170080000000002</v>
-      </c>
-      <c r="AI63" s="26">
-        <v>0.19961490000000001</v>
-      </c>
+      <c r="AI63" s="26"/>
       <c r="AO63" s="1">
         <v>0.23280149999999999</v>
       </c>
@@ -8897,7 +8887,7 @@
       </c>
       <c r="BI63" s="11"/>
     </row>
-    <row r="64" spans="1:61">
+    <row r="64" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A64" s="11">
         <v>94</v>
       </c>
@@ -8967,7 +8957,7 @@
       <c r="BH64" s="7"/>
       <c r="BI64" s="11"/>
     </row>
-    <row r="65" spans="1:61">
+    <row r="65" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A65" s="11">
         <v>51</v>
       </c>
@@ -8998,7 +8988,7 @@
       </c>
       <c r="BI65" s="11"/>
     </row>
-    <row r="66" spans="1:61">
+    <row r="66" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A66" s="11">
         <v>95</v>
       </c>
@@ -9030,7 +9020,7 @@
       <c r="BH66" s="7"/>
       <c r="BI66" s="11"/>
     </row>
-    <row r="67" spans="1:61">
+    <row r="67" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A67" s="11">
         <v>85</v>
       </c>
@@ -9071,7 +9061,7 @@
       <c r="BH67" s="7"/>
       <c r="BI67" s="11"/>
     </row>
-    <row r="68" spans="1:61">
+    <row r="68" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A68" s="11">
         <v>110</v>
       </c>
@@ -9099,7 +9089,7 @@
       <c r="BH68" s="7"/>
       <c r="BI68" s="11"/>
     </row>
-    <row r="69" spans="1:61">
+    <row r="69" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A69" s="11">
         <v>73</v>
       </c>
@@ -9171,7 +9161,7 @@
       </c>
       <c r="BI69" s="11"/>
     </row>
-    <row r="70" spans="1:61">
+    <row r="70" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A70" s="7">
         <v>73</v>
       </c>
@@ -9240,7 +9230,7 @@
       </c>
       <c r="BI70" s="7"/>
     </row>
-    <row r="71" spans="1:61">
+    <row r="71" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A71" s="11">
         <v>80</v>
       </c>
@@ -9268,7 +9258,7 @@
       <c r="BH71" s="7"/>
       <c r="BI71" s="11"/>
     </row>
-    <row r="72" spans="1:61">
+    <row r="72" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A72" s="11">
         <v>52</v>
       </c>
@@ -9296,7 +9286,7 @@
       <c r="BH72" s="7"/>
       <c r="BI72" s="11"/>
     </row>
-    <row r="73" spans="1:61">
+    <row r="73" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A73" s="11">
         <v>83</v>
       </c>
@@ -9366,7 +9356,7 @@
       <c r="BH73" s="7"/>
       <c r="BI73" s="11"/>
     </row>
-    <row r="74" spans="1:61">
+    <row r="74" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A74" s="11">
         <v>91</v>
       </c>
@@ -9441,7 +9431,7 @@
       </c>
       <c r="BI74" s="11"/>
     </row>
-    <row r="75" spans="1:61">
+    <row r="75" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A75" s="11">
         <v>72</v>
       </c>
@@ -9558,7 +9548,7 @@
       </c>
       <c r="BI75" s="11"/>
     </row>
-    <row r="76" spans="1:61">
+    <row r="76" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A76" s="11">
         <v>92</v>
       </c>
@@ -9627,7 +9617,7 @@
       </c>
       <c r="BI76" s="11"/>
     </row>
-    <row r="77" spans="1:61">
+    <row r="77" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A77" s="11">
         <v>58</v>
       </c>
@@ -9655,7 +9645,7 @@
       <c r="BH77" s="7"/>
       <c r="BI77" s="11"/>
     </row>
-    <row r="78" spans="1:61">
+    <row r="78" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A78" s="11">
         <v>44</v>
       </c>
@@ -9760,7 +9750,7 @@
       </c>
       <c r="BI78" s="11"/>
     </row>
-    <row r="79" spans="1:61">
+    <row r="79" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A79" s="11">
         <v>55</v>
       </c>
@@ -9788,7 +9778,7 @@
       <c r="BH79" s="7"/>
       <c r="BI79" s="11"/>
     </row>
-    <row r="80" spans="1:61">
+    <row r="80" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A80" s="11">
         <v>43</v>
       </c>
@@ -9816,7 +9806,7 @@
       <c r="BH80" s="7"/>
       <c r="BI80" s="11"/>
     </row>
-    <row r="81" spans="1:61">
+    <row r="81" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A81" s="11">
         <v>40</v>
       </c>
@@ -9924,7 +9914,7 @@
       </c>
       <c r="BI81" s="11"/>
     </row>
-    <row r="82" spans="1:61">
+    <row r="82" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A82" s="11">
         <v>81</v>
       </c>
@@ -9979,7 +9969,7 @@
       <c r="BH82" s="7"/>
       <c r="BI82" s="11"/>
     </row>
-    <row r="83" spans="1:61">
+    <row r="83" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A83" s="7">
         <v>81</v>
       </c>
@@ -10025,7 +10015,7 @@
       <c r="BH83" s="7"/>
       <c r="BI83" s="7"/>
     </row>
-    <row r="84" spans="1:61">
+    <row r="84" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A84" s="11">
         <v>59</v>
       </c>
@@ -10092,15 +10082,9 @@
       <c r="AF84" s="7">
         <v>0.92</v>
       </c>
-      <c r="AG84" s="26">
-        <v>0.24723990000000001</v>
-      </c>
-      <c r="AH84" s="26">
-        <v>0.2476749</v>
-      </c>
-      <c r="AI84" s="26">
-        <v>0.1364398</v>
-      </c>
+      <c r="AG84" s="26"/>
+      <c r="AH84" s="26"/>
+      <c r="AI84" s="26"/>
       <c r="AO84" s="26">
         <v>0.24723990000000001</v>
       </c>
@@ -10115,7 +10099,7 @@
       </c>
       <c r="BI84" s="11"/>
     </row>
-    <row r="85" spans="1:61">
+    <row r="85" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>108</v>
       </c>
@@ -10169,7 +10153,7 @@
       </c>
       <c r="BI85"/>
     </row>
-    <row r="86" spans="1:61">
+    <row r="86" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>105</v>
       </c>
@@ -10196,7 +10180,7 @@
       </c>
       <c r="BI86"/>
     </row>
-    <row r="87" spans="1:61">
+    <row r="87" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>62</v>
       </c>
@@ -10260,15 +10244,8 @@
       <c r="AA87" s="9">
         <v>0.74199999999999999</v>
       </c>
-      <c r="AG87" s="1">
-        <v>0.2628393</v>
-      </c>
-      <c r="AH87" s="26">
-        <v>0.30556129999999998</v>
-      </c>
-      <c r="AI87" s="26">
-        <v>0.27764349999999999</v>
-      </c>
+      <c r="AH87" s="26"/>
+      <c r="AI87" s="26"/>
       <c r="AO87" s="1">
         <v>0.2628393</v>
       </c>
@@ -10283,7 +10260,7 @@
       </c>
       <c r="BI87"/>
     </row>
-    <row r="88" spans="1:61">
+    <row r="88" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>101</v>
       </c>
@@ -10310,7 +10287,7 @@
       </c>
       <c r="BI88"/>
     </row>
-    <row r="89" spans="1:61">
+    <row r="89" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>76</v>
       </c>
@@ -10382,7 +10359,7 @@
       </c>
       <c r="BI89"/>
     </row>
-    <row r="90" spans="1:61">
+    <row r="90" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>76</v>
       </c>
@@ -10448,7 +10425,7 @@
       </c>
       <c r="BI90"/>
     </row>
-    <row r="91" spans="1:61">
+    <row r="91" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>76</v>
       </c>
@@ -10514,7 +10491,7 @@
       </c>
       <c r="BI91"/>
     </row>
-    <row r="92" spans="1:61">
+    <row r="92" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>76</v>
       </c>
@@ -10580,7 +10557,7 @@
       </c>
       <c r="BI92"/>
     </row>
-    <row r="93" spans="1:61">
+    <row r="93" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>76</v>
       </c>
@@ -10643,7 +10620,7 @@
       </c>
       <c r="BI93"/>
     </row>
-    <row r="94" spans="1:61">
+    <row r="94" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>76</v>
       </c>
@@ -10709,7 +10686,7 @@
       </c>
       <c r="BI94"/>
     </row>
-    <row r="95" spans="1:61">
+    <row r="95" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>76</v>
       </c>
@@ -10775,7 +10752,7 @@
       </c>
       <c r="BI95"/>
     </row>
-    <row r="96" spans="1:61">
+    <row r="96" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>42</v>
       </c>
@@ -10845,15 +10822,15 @@
       <c r="AD96" s="7">
         <v>0.23</v>
       </c>
-      <c r="AG96" s="26">
-        <v>0.1958955</v>
-      </c>
-      <c r="AH96" s="26">
-        <v>0.25844519999999999</v>
-      </c>
-      <c r="AI96" s="26">
-        <v>0.16113340000000001</v>
-      </c>
+      <c r="AE96" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="AF96" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="AG96" s="26"/>
+      <c r="AH96" s="26"/>
+      <c r="AI96" s="26"/>
       <c r="AJ96" s="9">
         <v>112.5</v>
       </c>
@@ -10874,7 +10851,7 @@
       </c>
       <c r="BI96"/>
     </row>
-    <row r="97" spans="1:61">
+    <row r="97" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>89</v>
       </c>
@@ -10943,7 +10920,7 @@
       </c>
       <c r="BI97"/>
     </row>
-    <row r="98" spans="1:61">
+    <row r="98" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>50</v>
       </c>
@@ -11069,7 +11046,7 @@
       </c>
       <c r="BI98"/>
     </row>
-    <row r="99" spans="1:61">
+    <row r="99" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>50</v>
       </c>
@@ -11185,7 +11162,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="100" spans="1:61">
+    <row r="100" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>112</v>
       </c>
@@ -11260,7 +11237,7 @@
       </c>
       <c r="BI100"/>
     </row>
-    <row r="101" spans="1:61">
+    <row r="101" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>112</v>
       </c>
@@ -11325,7 +11302,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="102" spans="1:61">
+    <row r="102" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>70</v>
       </c>
@@ -11391,7 +11368,7 @@
       </c>
       <c r="BI102"/>
     </row>
-    <row r="103" spans="1:61">
+    <row r="103" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>47</v>
       </c>
@@ -11415,7 +11392,7 @@
       </c>
       <c r="BI103"/>
     </row>
-    <row r="104" spans="1:61">
+    <row r="104" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -11529,7 +11506,7 @@
       </c>
       <c r="BI104"/>
     </row>
-    <row r="105" spans="1:61">
+    <row r="105" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>97</v>
       </c>
@@ -11619,7 +11596,7 @@
       </c>
       <c r="BI105"/>
     </row>
-    <row r="106" spans="1:61">
+    <row r="106" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>65</v>
       </c>
@@ -11766,7 +11743,7 @@
       </c>
       <c r="BI106"/>
     </row>
-    <row r="107" spans="1:61">
+    <row r="107" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A107" s="11">
         <v>113</v>
       </c>
@@ -11839,7 +11816,7 @@
       </c>
       <c r="BI107" s="11"/>
     </row>
-    <row r="108" spans="1:61">
+    <row r="108" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A108" s="11">
         <v>118</v>
       </c>
@@ -11923,7 +11900,7 @@
       </c>
       <c r="BI108" s="11"/>
     </row>
-    <row r="109" spans="1:61">
+    <row r="109" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A109" s="11">
         <v>118</v>
       </c>
@@ -12001,7 +11978,7 @@
       </c>
       <c r="BI109" s="7"/>
     </row>
-    <row r="110" spans="1:61">
+    <row r="110" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A110" s="11">
         <v>121</v>
       </c>
@@ -12065,15 +12042,9 @@
       <c r="AF110" s="7">
         <v>0.84</v>
       </c>
-      <c r="AG110" s="26">
-        <v>0.21827099999999999</v>
-      </c>
-      <c r="AH110" s="26">
-        <v>0.2890624</v>
-      </c>
-      <c r="AI110" s="7">
-        <v>0.2384077</v>
-      </c>
+      <c r="AG110" s="26"/>
+      <c r="AH110" s="26"/>
+      <c r="AI110" s="7"/>
       <c r="AO110" s="26">
         <v>0.21827099999999999</v>
       </c>
@@ -12091,7 +12062,7 @@
       </c>
       <c r="BI110" s="11"/>
     </row>
-    <row r="111" spans="1:61">
+    <row r="111" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A111" s="11">
         <v>115</v>
       </c>
@@ -12172,7 +12143,7 @@
       </c>
       <c r="BI111" s="11"/>
     </row>
-    <row r="112" spans="1:61">
+    <row r="112" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A112" s="11">
         <v>117</v>
       </c>
@@ -12271,7 +12242,7 @@
       </c>
       <c r="BI112" s="11"/>
     </row>
-    <row r="113" spans="1:61">
+    <row r="113" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A113" s="11">
         <v>116</v>
       </c>
@@ -12379,7 +12350,7 @@
       </c>
       <c r="BI113" s="11"/>
     </row>
-    <row r="114" spans="1:61">
+    <row r="114" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A114" s="11">
         <v>123</v>
       </c>
@@ -12460,7 +12431,7 @@
       </c>
       <c r="BI114" s="11"/>
     </row>
-    <row r="115" spans="1:61">
+    <row r="115" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A115" s="11">
         <v>119</v>
       </c>
@@ -12536,15 +12507,9 @@
       <c r="AF115" s="7">
         <v>0.83</v>
       </c>
-      <c r="AG115" s="7">
-        <v>0.23280149999999999</v>
-      </c>
-      <c r="AH115" s="7">
-        <v>0.27170080000000002</v>
-      </c>
-      <c r="AI115" s="7">
-        <v>0.19961490000000001</v>
-      </c>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
       <c r="AO115" s="7">
         <v>0.23280149999999999</v>
       </c>
@@ -12559,7 +12524,7 @@
       </c>
       <c r="BI115" s="11"/>
     </row>
-    <row r="116" spans="1:61">
+    <row r="116" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A116" s="11">
         <v>114</v>
       </c>
@@ -12641,7 +12606,7 @@
       </c>
       <c r="BI116" s="11"/>
     </row>
-    <row r="117" spans="1:61">
+    <row r="117" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A117" s="11">
         <v>114</v>
       </c>
@@ -12714,7 +12679,7 @@
       </c>
       <c r="BI117" s="11"/>
     </row>
-    <row r="118" spans="1:61">
+    <row r="118" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A118" s="11">
         <v>114</v>
       </c>
@@ -12787,7 +12752,7 @@
       </c>
       <c r="BI118" s="11"/>
     </row>
-    <row r="119" spans="1:61">
+    <row r="119" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A119" s="7">
         <v>114</v>
       </c>
@@ -12860,7 +12825,7 @@
       </c>
       <c r="BI119" s="7"/>
     </row>
-    <row r="120" spans="1:61">
+    <row r="120" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A120" s="11">
         <v>122</v>
       </c>
@@ -12932,7 +12897,7 @@
       </c>
       <c r="BI120" s="11"/>
     </row>
-    <row r="121" spans="1:61">
+    <row r="121" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A121" s="11">
         <v>120</v>
       </c>
@@ -12978,7 +12943,7 @@
       <c r="BH121" s="7"/>
       <c r="BI121" s="11"/>
     </row>
-    <row r="122" spans="1:61">
+    <row r="122" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>129</v>
       </c>
@@ -13065,7 +13030,7 @@
       </c>
       <c r="BI122"/>
     </row>
-    <row r="123" spans="1:61">
+    <row r="123" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>126</v>
       </c>
@@ -13170,7 +13135,7 @@
       </c>
       <c r="BI123"/>
     </row>
-    <row r="124" spans="1:61">
+    <row r="124" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>124</v>
       </c>
@@ -13246,15 +13211,9 @@
       <c r="AF124" s="7">
         <v>0.93</v>
       </c>
-      <c r="AG124" s="7">
-        <v>0.146394</v>
-      </c>
-      <c r="AH124" s="26">
-        <v>0.2219286</v>
-      </c>
-      <c r="AI124" s="7">
-        <v>0.13164390000000001</v>
-      </c>
+      <c r="AG124" s="7"/>
+      <c r="AH124" s="26"/>
+      <c r="AI124" s="7"/>
       <c r="AO124" s="7">
         <v>0.146394</v>
       </c>
@@ -13269,7 +13228,7 @@
       </c>
       <c r="BI124"/>
     </row>
-    <row r="125" spans="1:61">
+    <row r="125" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>131</v>
       </c>
@@ -13336,15 +13295,9 @@
       <c r="AF125" s="7">
         <v>0.85</v>
       </c>
-      <c r="AG125" s="7">
-        <v>0.21291959999999999</v>
-      </c>
-      <c r="AH125" s="26">
-        <v>0.27367229999999998</v>
-      </c>
-      <c r="AI125" s="26">
-        <v>0.1919208</v>
-      </c>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="26"/>
+      <c r="AI125" s="26"/>
       <c r="AO125" s="7">
         <v>0.21291959999999999</v>
       </c>
@@ -13359,7 +13312,7 @@
       </c>
       <c r="BI125"/>
     </row>
-    <row r="126" spans="1:61">
+    <row r="126" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -13449,7 +13402,7 @@
       </c>
       <c r="BI126"/>
     </row>
-    <row r="127" spans="1:61">
+    <row r="127" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>127</v>
       </c>
@@ -13536,7 +13489,7 @@
       </c>
       <c r="BI127"/>
     </row>
-    <row r="128" spans="1:61">
+    <row r="128" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>129</v>
       </c>
@@ -13586,9 +13539,9 @@
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1">
+    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1037</v>
       </c>
@@ -13613,7 +13566,7 @@
       <c r="AJ1" s="9"/>
       <c r="AO1" s="4"/>
     </row>
-    <row r="2" spans="1:45" s="1" customFormat="1">
+    <row r="2" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>414</v>
       </c>
@@ -13635,7 +13588,7 @@
       <c r="AJ2" s="9"/>
       <c r="AS2" s="4"/>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -13644,7 +13597,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -13653,7 +13606,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -13662,7 +13615,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -13671,7 +13624,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>430</v>
       </c>
@@ -13682,7 +13635,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -13693,7 +13646,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1119</v>
       </c>
@@ -13704,7 +13657,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -13715,7 +13668,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1047</v>
       </c>
@@ -13726,7 +13679,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -13737,7 +13690,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -13748,7 +13701,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -13759,7 +13712,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>494</v>
       </c>
@@ -13770,7 +13723,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>410</v>
       </c>
@@ -13781,7 +13734,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>402</v>
       </c>
@@ -13792,7 +13745,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>401</v>
       </c>
@@ -13803,7 +13756,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -13814,7 +13767,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -13825,7 +13778,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -13834,7 +13787,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -13843,7 +13796,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
@@ -13854,7 +13807,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>1067</v>
       </c>
@@ -13865,7 +13818,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>1071</v>
       </c>
@@ -13876,7 +13829,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
@@ -13887,7 +13840,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>1068</v>
       </c>
@@ -13898,7 +13851,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>1072</v>
       </c>
@@ -13909,7 +13862,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>22</v>
       </c>
@@ -13920,7 +13873,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>1069</v>
       </c>
@@ -13931,7 +13884,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>1073</v>
       </c>
@@ -13942,7 +13895,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>17</v>
       </c>
@@ -13953,7 +13906,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>15</v>
       </c>
@@ -13962,7 +13915,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>16</v>
       </c>
@@ -13971,7 +13924,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>392</v>
       </c>
@@ -13979,7 +13932,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>393</v>
       </c>
@@ -13988,7 +13941,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>394</v>
       </c>
@@ -13997,7 +13950,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>98</v>
       </c>
@@ -14008,7 +13961,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>1088</v>
       </c>
@@ -14019,7 +13972,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>1070</v>
       </c>
@@ -14028,7 +13981,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -14039,7 +13992,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>400</v>
       </c>
@@ -14050,7 +14003,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>1211</v>
       </c>
@@ -14059,7 +14012,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -14070,7 +14023,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>701</v>
       </c>
@@ -14081,7 +14034,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>708</v>
       </c>
@@ -14092,7 +14045,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>709</v>
       </c>
@@ -14101,7 +14054,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>705</v>
       </c>
@@ -14112,7 +14065,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>706</v>
       </c>
@@ -14121,7 +14074,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>711</v>
       </c>
@@ -14130,7 +14083,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>712</v>
       </c>
@@ -14139,7 +14092,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>713</v>
       </c>
@@ -14148,7 +14101,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>714</v>
       </c>
@@ -14157,7 +14110,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>1110</v>
       </c>
@@ -14168,7 +14121,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>1111</v>
       </c>
@@ -14179,7 +14132,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>1112</v>
       </c>
@@ -14190,7 +14143,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>1113</v>
       </c>
@@ -14201,7 +14154,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>1114</v>
       </c>
@@ -14212,7 +14165,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>1115</v>
       </c>
@@ -14236,9 +14189,9 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>906</v>
       </c>
@@ -14273,7 +14226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>907</v>
       </c>
@@ -14305,7 +14258,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>908</v>
       </c>
@@ -14331,7 +14284,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>909</v>
       </c>
@@ -14364,7 +14317,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>910</v>
       </c>
@@ -14397,7 +14350,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>911</v>
       </c>
@@ -14426,7 +14379,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>912</v>
       </c>
@@ -14459,7 +14412,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>913</v>
       </c>
@@ -14491,7 +14444,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>914</v>
       </c>
@@ -14520,7 +14473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>915</v>
       </c>
@@ -14549,7 +14502,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>916</v>
       </c>
@@ -14579,7 +14532,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>917</v>
       </c>
@@ -14611,7 +14564,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>926</v>
       </c>
@@ -14640,7 +14593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>918</v>
       </c>
@@ -14669,7 +14622,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>919</v>
       </c>
@@ -14698,7 +14651,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>920</v>
       </c>
@@ -14727,7 +14680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>921</v>
       </c>
@@ -14757,7 +14710,7 @@
         <v>3.3557046979865772E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>1148</v>
       </c>
@@ -14787,7 +14740,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>922</v>
       </c>
@@ -14817,7 +14770,7 @@
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>923</v>
       </c>
@@ -14847,7 +14800,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>924</v>
       </c>
@@ -14880,7 +14833,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>925</v>
       </c>
@@ -14909,7 +14862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>1142</v>
       </c>
@@ -14938,7 +14891,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>984</v>
       </c>
@@ -14967,7 +14920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1175</v>
       </c>
@@ -14997,7 +14950,7 @@
         <v>6.9767441860465115E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>46</v>
       </c>
@@ -15027,7 +14980,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1189</v>
       </c>
@@ -15060,7 +15013,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1182</v>
       </c>
@@ -15092,7 +15045,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>1182</v>
       </c>
@@ -15121,7 +15074,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>1182</v>
       </c>
@@ -15165,9 +15118,9 @@
       <selection activeCell="B11" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1116</v>
       </c>
@@ -15175,12 +15128,12 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -15188,7 +15141,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>939</v>
       </c>
@@ -15196,7 +15149,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -15204,7 +15157,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1119</v>
       </c>
@@ -15212,7 +15165,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -15220,7 +15173,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -15228,7 +15181,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>929</v>
       </c>
@@ -15236,7 +15189,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>928</v>
       </c>
@@ -15244,7 +15197,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -15265,7 +15218,7 @@
       <selection activeCell="B2" sqref="B2:B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="66.83203125" bestFit="1" customWidth="1"/>
@@ -15276,7 +15229,7 @@
     <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>381</v>
       </c>
@@ -15304,7 +15257,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>100</v>
       </c>
@@ -15336,7 +15289,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>49</v>
       </c>
@@ -15368,7 +15321,7 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>60</v>
       </c>
@@ -15400,7 +15353,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>77</v>
       </c>
@@ -15430,7 +15383,7 @@
         <v>3539</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>69</v>
       </c>
@@ -15462,7 +15415,7 @@
         <v>4234</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>109</v>
       </c>
@@ -15494,7 +15447,7 @@
         <v>5638</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>46</v>
       </c>
@@ -15526,7 +15479,7 @@
         <v>6122</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>84</v>
       </c>
@@ -15558,7 +15511,7 @@
         <v>9224</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>63</v>
       </c>
@@ -15590,7 +15543,7 @@
         <v>10433</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>74</v>
       </c>
@@ -15622,7 +15575,7 @@
         <v>11099</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>107</v>
       </c>
@@ -15654,7 +15607,7 @@
         <v>12231</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>71</v>
       </c>
@@ -15686,7 +15639,7 @@
         <v>12551</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>113</v>
       </c>
@@ -15718,7 +15671,7 @@
         <v>12642</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>66</v>
       </c>
@@ -15750,7 +15703,7 @@
         <v>13436</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>53</v>
       </c>
@@ -15782,7 +15735,7 @@
         <v>13645</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>75</v>
       </c>
@@ -15814,7 +15767,7 @@
         <v>20018</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>54</v>
       </c>
@@ -15846,7 +15799,7 @@
         <v>20324</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="2" customFormat="1">
+    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>102</v>
       </c>
@@ -15874,7 +15827,7 @@
         <v>25297</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1">
+    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>90</v>
       </c>
@@ -15906,7 +15859,7 @@
         <v>26913</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="2" customFormat="1">
+    <row r="21" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>61</v>
       </c>
@@ -15934,7 +15887,7 @@
         <v>28649</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="2" customFormat="1">
+    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>86</v>
       </c>
@@ -15966,7 +15919,7 @@
         <v>29155</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="2" customFormat="1">
+    <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
         <v>57</v>
       </c>
@@ -15996,7 +15949,7 @@
         <v>32758</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="2" customFormat="1">
+    <row r="24" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>78</v>
       </c>
@@ -16028,7 +15981,7 @@
         <v>32791</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="2" customFormat="1">
+    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
         <v>64</v>
       </c>
@@ -16060,7 +16013,7 @@
         <v>32959</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="2" customFormat="1">
+    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>68</v>
       </c>
@@ -16092,7 +16045,7 @@
         <v>34746</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="2" customFormat="1">
+    <row r="27" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>93</v>
       </c>
@@ -16124,7 +16077,7 @@
         <v>37672</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1">
+    <row r="28" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>48</v>
       </c>
@@ -16156,7 +16109,7 @@
         <v>38933</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="2" customFormat="1">
+    <row r="29" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>88</v>
       </c>
@@ -16188,7 +16141,7 @@
         <v>39237</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="2" customFormat="1">
+    <row r="30" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>111</v>
       </c>
@@ -16220,7 +16173,7 @@
         <v>39944</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="2" customFormat="1">
+    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>56</v>
       </c>
@@ -16252,7 +16205,7 @@
         <v>41100</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="2" customFormat="1">
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>82</v>
       </c>
@@ -16284,7 +16237,7 @@
         <v>41932</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="2" customFormat="1">
+    <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>104</v>
       </c>
@@ -16316,7 +16269,7 @@
         <v>46216</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="2" customFormat="1">
+    <row r="34" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>87</v>
       </c>
@@ -16346,7 +16299,7 @@
         <v>46967</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="2" customFormat="1">
+    <row r="35" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>45</v>
       </c>
@@ -16378,7 +16331,7 @@
         <v>47378</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="2" customFormat="1">
+    <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>67</v>
       </c>
@@ -16410,7 +16363,7 @@
         <v>48354</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="2" customFormat="1">
+    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>96</v>
       </c>
@@ -16442,7 +16395,7 @@
         <v>49003</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="2" customFormat="1">
+    <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>98</v>
       </c>
@@ -16474,7 +16427,7 @@
         <v>50537</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="2" customFormat="1">
+    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>79</v>
       </c>
@@ -16506,7 +16459,7 @@
         <v>50542</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="2" customFormat="1">
+    <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>41</v>
       </c>
@@ -16538,7 +16491,7 @@
         <v>50721</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="2" customFormat="1">
+    <row r="41" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11">
         <v>106</v>
       </c>
@@ -16570,7 +16523,7 @@
         <v>51750</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="2" customFormat="1">
+    <row r="42" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>99</v>
       </c>
@@ -16602,7 +16555,7 @@
         <v>52971</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="2" customFormat="1">
+    <row r="43" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11">
         <v>94</v>
       </c>
@@ -16634,7 +16587,7 @@
         <v>54361</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="2" customFormat="1">
+    <row r="44" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>51</v>
       </c>
@@ -16666,7 +16619,7 @@
         <v>54775</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="2" customFormat="1">
+    <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>95</v>
       </c>
@@ -16698,7 +16651,7 @@
         <v>54968</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="2" customFormat="1">
+    <row r="46" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>85</v>
       </c>
@@ -16730,7 +16683,7 @@
         <v>55220</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="2" customFormat="1">
+    <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
         <v>110</v>
       </c>
@@ -16762,7 +16715,7 @@
         <v>56086</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="2" customFormat="1">
+    <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>73</v>
       </c>
@@ -16794,7 +16747,7 @@
         <v>56525</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="2" customFormat="1">
+    <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
         <v>80</v>
       </c>
@@ -16826,7 +16779,7 @@
         <v>57840</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="2" customFormat="1">
+    <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
         <v>52</v>
       </c>
@@ -16858,7 +16811,7 @@
         <v>58896</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
         <v>83</v>
       </c>
@@ -16890,7 +16843,7 @@
         <v>59284</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>91</v>
       </c>
@@ -16922,7 +16875,7 @@
         <v>59320</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
         <v>72</v>
       </c>
@@ -16954,7 +16907,7 @@
         <v>60703</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
         <v>92</v>
       </c>
@@ -16986,7 +16939,7 @@
         <v>66679</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
         <v>58</v>
       </c>
@@ -17016,7 +16969,7 @@
         <v>67037</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>44</v>
       </c>
@@ -17048,7 +17001,7 @@
         <v>73767</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
         <v>55</v>
       </c>
@@ -17080,7 +17033,7 @@
         <v>73924</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="11">
         <v>43</v>
       </c>
@@ -17112,7 +17065,7 @@
         <v>74887</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="11">
         <v>40</v>
       </c>
@@ -17142,7 +17095,7 @@
         <v>75330</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="11">
         <v>81</v>
       </c>
@@ -17172,7 +17125,7 @@
         <v>76460</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -17204,7 +17157,7 @@
         <v>78680</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
         <v>108</v>
       </c>
@@ -17236,7 +17189,7 @@
         <v>80275</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="11">
         <v>105</v>
       </c>
@@ -17268,7 +17221,7 @@
         <v>81054</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -17300,7 +17253,7 @@
         <v>81684</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="11">
         <v>101</v>
       </c>
@@ -17332,7 +17285,7 @@
         <v>82696</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="11">
         <v>76</v>
       </c>
@@ -17360,7 +17313,7 @@
         <v>83890</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="11">
         <v>42</v>
       </c>
@@ -17392,7 +17345,7 @@
         <v>84689</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="11">
         <v>89</v>
       </c>
@@ -17424,7 +17377,7 @@
         <v>88432</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="11">
         <v>50</v>
       </c>
@@ -17456,7 +17409,7 @@
         <v>89054</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="11">
         <v>112</v>
       </c>
@@ -17488,7 +17441,7 @@
         <v>90316</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="11">
         <v>70</v>
       </c>
@@ -17520,7 +17473,7 @@
         <v>92735</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="11">
         <v>47</v>
       </c>
@@ -17552,7 +17505,7 @@
         <v>93418</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="11">
         <v>103</v>
       </c>
@@ -17582,7 +17535,7 @@
         <v>94860</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="11">
         <v>97</v>
       </c>
@@ -17614,7 +17567,7 @@
         <v>95244</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="11">
         <v>65</v>
       </c>
@@ -17663,9 +17616,9 @@
       <selection activeCell="B12" activeCellId="1" sqref="B15:B21 B2:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>381</v>
       </c>
@@ -17685,7 +17638,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>113</v>
       </c>
@@ -17705,7 +17658,7 @@
         <v>2.0152920465801638E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>118</v>
       </c>
@@ -17725,7 +17678,7 @@
         <v>4.674181240213704E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>121</v>
       </c>
@@ -17745,7 +17698,7 @@
         <v>0.13282679210562631</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>115</v>
       </c>
@@ -17765,7 +17718,7 @@
         <v>0.14772978119295221</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>117</v>
       </c>
@@ -17785,7 +17738,7 @@
         <v>0.19497116776968848</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>116</v>
       </c>
@@ -17805,7 +17758,7 @@
         <v>0.3082658551556392</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>123</v>
       </c>
@@ -17825,7 +17778,7 @@
         <v>0.35522680376280447</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>119</v>
       </c>
@@ -17845,7 +17798,7 @@
         <v>0.51238651611118913</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>114</v>
       </c>
@@ -17865,7 +17818,7 @@
         <v>0.79962543936843022</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>122</v>
       </c>
@@ -17885,7 +17838,7 @@
         <v>0.82351857412982277</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>120</v>
       </c>
@@ -17905,7 +17858,7 @@
         <v>0.91283573016383235</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>979</v>
       </c>
@@ -17913,7 +17866,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>130</v>
       </c>
@@ -17927,7 +17880,7 @@
         <v>4.5647988135790185E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>126</v>
       </c>
@@ -17941,7 +17894,7 @@
         <v>0.19975369256546105</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>124</v>
       </c>
@@ -17955,7 +17908,7 @@
         <v>0.38904191938792043</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>131</v>
       </c>
@@ -17969,7 +17922,7 @@
         <v>0.46913668197324998</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>125</v>
       </c>
@@ -17983,7 +17936,7 @@
         <v>0.47343686143616748</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>127</v>
       </c>
@@ -17997,7 +17950,7 @@
         <v>0.66023299344219599</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>129</v>
       </c>
@@ -18028,9 +17981,9 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>906</v>
       </c>
@@ -18041,7 +17994,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>907</v>
       </c>
@@ -18052,7 +18005,7 @@
         <v>0.11780915591189201</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>908</v>
       </c>
@@ -18063,7 +18016,7 @@
         <v>0.14190518438276789</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>909</v>
       </c>
@@ -18074,7 +18027,7 @@
         <v>0.15248178171981241</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>910</v>
       </c>
@@ -18085,7 +18038,7 @@
         <v>0.32424885057540331</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>911</v>
       </c>
@@ -18096,7 +18049,7 @@
         <v>0.36008942414901568</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>912</v>
       </c>
@@ -18107,7 +18060,7 @@
         <v>0.36473888979125946</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>913</v>
       </c>
@@ -18118,7 +18071,7 @@
         <v>0.37305006993859302</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>914</v>
       </c>
@@ -18129,7 +18082,7 @@
         <v>0.40549141682361001</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>915</v>
       </c>
@@ -18140,7 +18093,7 @@
         <v>0.49010771135660791</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>916</v>
       </c>
@@ -18151,7 +18104,7 @@
         <v>0.49766661039234461</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>917</v>
       </c>
@@ -18162,7 +18115,7 @@
         <v>0.53613889700361461</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>926</v>
       </c>
@@ -18173,7 +18126,7 @@
         <v>0.55372046150480514</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>918</v>
       </c>
@@ -18184,7 +18137,7 @@
         <v>0.56166742077086174</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>919</v>
       </c>
@@ -18195,7 +18148,7 @@
         <v>0.69538024858540026</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>920</v>
       </c>
@@ -18206,7 +18159,7 @@
         <v>0.72399036878219081</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>921</v>
       </c>
@@ -18217,7 +18170,7 @@
         <v>0.75372671693079174</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>922</v>
       </c>
@@ -18228,7 +18181,7 @@
         <v>0.90783927973393885</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>923</v>
       </c>
@@ -18239,7 +18192,7 @@
         <v>0.92374386939225039</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>924</v>
       </c>
@@ -18250,7 +18203,7 @@
         <v>0.979161553110653</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>925</v>
       </c>
@@ -18278,12 +18231,12 @@
       <selection activeCell="B1" sqref="B1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.20703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>1200</v>
       </c>
@@ -18297,7 +18250,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="21">
         <v>42989</v>
       </c>
@@ -18311,7 +18264,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="21">
         <v>42989</v>
       </c>
@@ -18325,7 +18278,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="21">
         <v>42989</v>
       </c>
@@ -18337,7 +18290,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="21">
         <v>42989</v>
       </c>
@@ -18351,16 +18304,16 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="19"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="20"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="20"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding in estiamtions of the SDs and Means from articles that do not provide.
</commit_message>
<xml_diff>
--- a/PowerEstimationReviewDataCollection2018.03.25.xlsx
+++ b/PowerEstimationReviewDataCollection2018.03.25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Systematic Reviews\History of Power Estimation Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6C8140-E504-44AB-9DC3-240A93C6942B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EAA8D8-6816-4D0C-96E3-DE43408C031A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="10640" windowHeight="5720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="1219">
   <si>
     <t>Author</t>
   </si>
@@ -3765,6 +3765,12 @@
   </si>
   <si>
     <t>SDLargeAlgEstFromCDT</t>
+  </si>
+  <si>
+    <t>Exclude (unclear how many articles at any level)</t>
+  </si>
+  <si>
+    <t>Unclear how many articles at each level</t>
   </si>
 </sst>
 </file>
@@ -4244,9 +4250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="39" zoomScaleNormal="47" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="39" zoomScaleNormal="47" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI26" sqref="AI26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6385,7 +6391,7 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="AI26" s="1">
-        <v>167</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="BI26" s="11"/>
     </row>
@@ -12540,6 +12546,9 @@
       <c r="E116" s="11">
         <v>1973</v>
       </c>
+      <c r="F116" s="7" t="s">
+        <v>1217</v>
+      </c>
       <c r="G116" s="18" t="s">
         <v>893</v>
       </c>
@@ -12601,6 +12610,9 @@
       <c r="AI116" s="7">
         <v>0.04</v>
       </c>
+      <c r="AR116" s="1" t="s">
+        <v>1218</v>
+      </c>
       <c r="AS116" s="1" t="s">
         <v>888</v>
       </c>
@@ -12616,6 +12628,9 @@
       <c r="E117" s="11">
         <v>1973</v>
       </c>
+      <c r="F117" s="7" t="s">
+        <v>1217</v>
+      </c>
       <c r="G117" s="18" t="s">
         <v>893</v>
       </c>
@@ -12677,6 +12692,9 @@
       <c r="AI117" s="7">
         <v>0.9</v>
       </c>
+      <c r="AR117" s="1" t="s">
+        <v>1218</v>
+      </c>
       <c r="BI117" s="11"/>
     </row>
     <row r="118" spans="1:61" x14ac:dyDescent="0.35">
@@ -12689,6 +12707,9 @@
       <c r="E118" s="11">
         <v>1973</v>
       </c>
+      <c r="F118" s="7" t="s">
+        <v>1217</v>
+      </c>
       <c r="G118" s="18" t="s">
         <v>893</v>
       </c>
@@ -12750,6 +12771,9 @@
       <c r="AI118" s="7">
         <v>0.05</v>
       </c>
+      <c r="AR118" s="1" t="s">
+        <v>1218</v>
+      </c>
       <c r="BI118" s="11"/>
     </row>
     <row r="119" spans="1:61" x14ac:dyDescent="0.35">
@@ -12762,6 +12786,9 @@
       <c r="E119" s="11">
         <v>1973</v>
       </c>
+      <c r="F119" s="7" t="s">
+        <v>1217</v>
+      </c>
       <c r="G119" s="18" t="s">
         <v>893</v>
       </c>
@@ -12822,6 +12849,9 @@
       </c>
       <c r="AI119" s="7">
         <v>0.11</v>
+      </c>
+      <c r="AR119" s="1" t="s">
+        <v>1218</v>
       </c>
       <c r="BI119" s="7"/>
     </row>

</xml_diff>

<commit_message>
Suplementary materials added and estimated
</commit_message>
<xml_diff>
--- a/PowerEstimationReviewDataCollection2018.03.25.xlsx
+++ b/PowerEstimationReviewDataCollection2018.03.25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Systematic Reviews\History of Power Estimation Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BA8B15-BC58-4850-A18A-E780B8998994}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98AAA01-7D46-49F5-95A4-55CEC241CE06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="465" windowWidth="10635" windowHeight="5715" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_power_estimates" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_Hlk504467761" localSheetId="7">'Search terms'!$A$1</definedName>
     <definedName name="PowerEstimationStudiesLib_for_export" localSheetId="4">Randomisation_original_sample!$A$2:$I$75</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,6 +36,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2505" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="1301">
   <si>
     <t>Author</t>
   </si>
@@ -3894,6 +3895,129 @@
   </si>
   <si>
     <t>Binary for reasons to have excluded articles - full text not available</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/002246698802200302</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/h0045186</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/01443410701491718</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/geront/20.4.494</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/j.1556-6978.1974.tb00854.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2307/1161755</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/10671188.1972.10615106</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1460-2466.1973.tb00947.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/0165-1781(81)90072-X</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/03637757509375874</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/0021-9924(75)90016-7</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/0021-9010.61.2.234</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/107769907605300217</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/10671315.1977.10762173</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/tea.3660200708</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2307/3150969</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/swra/22.3.3</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1086/644403</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1097/00001888-198309000-00005</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/smj.4250080410</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2307/256280</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037//0033-2909.105.2.309</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037//0894-4105.14.2.233</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/0021-9010.90.1.94</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037//0022-006X.68.1.166</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0033-3182(92)71948-3</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/00986280902739743</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1744-6570.1996.tb01793.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.2044-8295.1997.tb02621.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/1094428104263676</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2308/bria.2001.13.1.63</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037//0278-6133.20.1.76</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1440-1819.2011.02208.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1076/jcen.23.3.399.1181</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/13854040500203290</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5406/bulcouresmusedu.201.0043</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.psychsport.2015.11.005</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/071530</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>Binary for reasons to have excluded articles - article examines studies not in scope of literature review</t>
+  </si>
+  <si>
+    <t>DistinguishedStatisticalTestsAppropriately</t>
   </si>
 </sst>
 </file>
@@ -4023,7 +4147,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4037,8 +4161,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4091,8 +4216,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4105,6 +4231,7 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4387,51 +4514,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ128"/>
+  <dimension ref="A1:BI128"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="BF1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP1" sqref="AP1:AR1"/>
+      <selection pane="bottomLeft" activeCell="BI1" sqref="BI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="10.875" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="47.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="32.125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="5.625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="32.08203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5.58203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.08203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.58203125" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.75" style="1" customWidth="1"/>
     <col min="19" max="19" width="15.75" style="1" customWidth="1"/>
-    <col min="20" max="20" width="12.875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" style="1" customWidth="1"/>
     <col min="21" max="21" width="11.75" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.875" style="9" customWidth="1"/>
-    <col min="23" max="24" width="10.875" style="7" customWidth="1"/>
-    <col min="25" max="25" width="10.875" style="9" customWidth="1"/>
-    <col min="26" max="27" width="10.875" style="7" customWidth="1"/>
-    <col min="28" max="28" width="10.875" style="9" customWidth="1"/>
-    <col min="29" max="33" width="10.875" style="7" customWidth="1"/>
-    <col min="34" max="36" width="10.875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10.875" style="9" customWidth="1"/>
-    <col min="38" max="44" width="10.875" style="1" customWidth="1"/>
-    <col min="45" max="45" width="10.875" style="1"/>
-    <col min="46" max="54" width="10.875" style="1" customWidth="1"/>
-    <col min="55" max="60" width="10.875" style="1"/>
-    <col min="61" max="61" width="41.875" style="1" customWidth="1"/>
-    <col min="62" max="16384" width="10.875" style="1"/>
+    <col min="22" max="22" width="14.83203125" style="9" customWidth="1"/>
+    <col min="23" max="24" width="10.83203125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" style="9" customWidth="1"/>
+    <col min="26" max="27" width="10.83203125" style="7" customWidth="1"/>
+    <col min="28" max="28" width="10.83203125" style="9" customWidth="1"/>
+    <col min="29" max="33" width="10.83203125" style="7" customWidth="1"/>
+    <col min="34" max="36" width="10.83203125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="10.83203125" style="9" customWidth="1"/>
+    <col min="38" max="44" width="10.83203125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="10.83203125" style="1"/>
+    <col min="46" max="54" width="10.83203125" style="1" customWidth="1"/>
+    <col min="55" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62">
+    <row r="1" spans="1:61">
       <c r="A1" s="1" t="s">
         <v>401</v>
       </c>
@@ -4612,8 +4737,11 @@
       <c r="BH1" s="1" t="s">
         <v>1067</v>
       </c>
-    </row>
-    <row r="2" spans="1:62">
+      <c r="BI1" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61">
       <c r="A2" s="1">
         <v>100</v>
       </c>
@@ -4643,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:61">
       <c r="A3" s="1">
         <v>49</v>
       </c>
@@ -4736,7 +4864,7 @@
       </c>
       <c r="AW3" s="4"/>
     </row>
-    <row r="4" spans="1:62">
+    <row r="4" spans="1:61">
       <c r="A4" s="1">
         <v>49</v>
       </c>
@@ -4805,7 +4933,7 @@
       </c>
       <c r="AW4" s="4"/>
     </row>
-    <row r="5" spans="1:62">
+    <row r="5" spans="1:61">
       <c r="A5" s="7">
         <v>60</v>
       </c>
@@ -4915,9 +5043,9 @@
         <v>477</v>
       </c>
       <c r="AW5" s="4"/>
-      <c r="BJ5" s="7"/>
-    </row>
-    <row r="6" spans="1:62">
+      <c r="BI5" s="7"/>
+    </row>
+    <row r="6" spans="1:61">
       <c r="A6" s="1">
         <v>77</v>
       </c>
@@ -5018,8 +5146,11 @@
         <v>462</v>
       </c>
       <c r="AW6" s="4"/>
-    </row>
-    <row r="7" spans="1:62">
+      <c r="BI6" s="1" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61">
       <c r="A7" s="1">
         <v>77</v>
       </c>
@@ -5107,7 +5238,7 @@
       <c r="AS7" s="4"/>
       <c r="AW7" s="4"/>
     </row>
-    <row r="8" spans="1:62">
+    <row r="8" spans="1:61">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -5195,7 +5326,7 @@
       <c r="AS8" s="4"/>
       <c r="AW8" s="4"/>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:61">
       <c r="A9" s="1">
         <v>77</v>
       </c>
@@ -5283,7 +5414,7 @@
       <c r="AS9" s="4"/>
       <c r="AW9" s="4"/>
     </row>
-    <row r="10" spans="1:62">
+    <row r="10" spans="1:61">
       <c r="A10" s="1">
         <v>77</v>
       </c>
@@ -5371,7 +5502,7 @@
       <c r="AS10" s="4"/>
       <c r="AW10" s="4"/>
     </row>
-    <row r="11" spans="1:62">
+    <row r="11" spans="1:61">
       <c r="A11" s="1">
         <v>69</v>
       </c>
@@ -5469,7 +5600,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="12" spans="1:62">
+    <row r="12" spans="1:61">
       <c r="A12" s="1">
         <v>69</v>
       </c>
@@ -5561,7 +5692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:62">
+    <row r="13" spans="1:61">
       <c r="A13" s="1">
         <v>69</v>
       </c>
@@ -5653,7 +5784,7 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="14" spans="1:62">
+    <row r="14" spans="1:61">
       <c r="A14" s="1">
         <v>109</v>
       </c>
@@ -5727,7 +5858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:62">
+    <row r="15" spans="1:61">
       <c r="A15" s="1">
         <v>46</v>
       </c>
@@ -5756,7 +5887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:62">
+    <row r="16" spans="1:61">
       <c r="A16" s="1">
         <v>84</v>
       </c>
@@ -5785,7 +5916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:62">
+    <row r="17" spans="1:61">
       <c r="A17" s="1">
         <v>63</v>
       </c>
@@ -5850,7 +5981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:62">
+    <row r="18" spans="1:61">
       <c r="A18" s="1">
         <v>74</v>
       </c>
@@ -5945,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:62">
+    <row r="19" spans="1:61">
       <c r="A19" s="1">
         <v>107</v>
       </c>
@@ -6060,8 +6191,11 @@
       <c r="AM19" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:62">
+      <c r="BI19" s="1" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:61">
       <c r="A20" s="1">
         <v>71</v>
       </c>
@@ -6185,8 +6319,11 @@
       <c r="AS20" s="1" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="21" spans="1:62">
+      <c r="BI20" s="1" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:61">
       <c r="A21" s="1">
         <v>113</v>
       </c>
@@ -6257,7 +6394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:62">
+    <row r="22" spans="1:61">
       <c r="A22" s="1">
         <v>66</v>
       </c>
@@ -6343,7 +6480,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="23" spans="1:62">
+    <row r="23" spans="1:61">
       <c r="A23" s="1">
         <v>53</v>
       </c>
@@ -6372,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:62">
+    <row r="24" spans="1:61">
       <c r="A24" s="1">
         <v>75</v>
       </c>
@@ -6463,8 +6600,11 @@
       <c r="AS24" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="25" spans="1:62">
+      <c r="BI24" s="1" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:61">
       <c r="A25" s="1">
         <v>54</v>
       </c>
@@ -6514,7 +6654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:62">
+    <row r="26" spans="1:61">
       <c r="A26" s="11">
         <v>102</v>
       </c>
@@ -6620,9 +6760,9 @@
       <c r="AJ26" s="1">
         <v>0.16700000000000001</v>
       </c>
-      <c r="BJ26" s="11"/>
-    </row>
-    <row r="27" spans="1:62">
+      <c r="BI26" s="11"/>
+    </row>
+    <row r="27" spans="1:61">
       <c r="A27" s="11">
         <v>90</v>
       </c>
@@ -6662,10 +6802,9 @@
       <c r="BF27" s="1">
         <v>1</v>
       </c>
-      <c r="BI27" s="7"/>
-      <c r="BJ27" s="11"/>
-    </row>
-    <row r="28" spans="1:62">
+      <c r="BI27" s="11"/>
+    </row>
+    <row r="28" spans="1:61">
       <c r="A28" s="11">
         <v>61</v>
       </c>
@@ -6708,10 +6847,9 @@
       <c r="BE28" s="1">
         <v>1</v>
       </c>
-      <c r="BI28" s="7"/>
-      <c r="BJ28" s="11"/>
-    </row>
-    <row r="29" spans="1:62">
+      <c r="BI28" s="11"/>
+    </row>
+    <row r="29" spans="1:61">
       <c r="A29" s="11">
         <v>86</v>
       </c>
@@ -6799,9 +6937,11 @@
       <c r="AJ29" s="1">
         <v>0.18</v>
       </c>
-      <c r="BJ29" s="11"/>
-    </row>
-    <row r="30" spans="1:62">
+      <c r="BI29" s="11" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:61">
       <c r="A30" s="11">
         <v>57</v>
       </c>
@@ -6877,10 +7017,9 @@
       <c r="BE30" s="1">
         <v>1</v>
       </c>
-      <c r="BI30" s="7"/>
-      <c r="BJ30" s="11"/>
-    </row>
-    <row r="31" spans="1:62">
+      <c r="BI30" s="11"/>
+    </row>
+    <row r="31" spans="1:61">
       <c r="A31" s="11">
         <v>57</v>
       </c>
@@ -6947,10 +7086,9 @@
       <c r="AS31" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="BI31" s="7"/>
-      <c r="BJ31" s="11"/>
-    </row>
-    <row r="32" spans="1:62">
+      <c r="BI31" s="11"/>
+    </row>
+    <row r="32" spans="1:61">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -7018,10 +7156,9 @@
       <c r="AS32" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="BI32" s="7"/>
-      <c r="BJ32" s="11"/>
-    </row>
-    <row r="33" spans="1:62">
+      <c r="BI32" s="11"/>
+    </row>
+    <row r="33" spans="1:61">
       <c r="A33" s="11">
         <v>57</v>
       </c>
@@ -7089,10 +7226,9 @@
       <c r="AS33" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="BI33" s="7"/>
-      <c r="BJ33" s="11"/>
-    </row>
-    <row r="34" spans="1:62">
+      <c r="BI33" s="11"/>
+    </row>
+    <row r="34" spans="1:61">
       <c r="A34" s="11">
         <v>57</v>
       </c>
@@ -7160,10 +7296,9 @@
       <c r="AS34" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="BI34" s="7"/>
-      <c r="BJ34" s="11"/>
-    </row>
-    <row r="35" spans="1:62">
+      <c r="BI34" s="11"/>
+    </row>
+    <row r="35" spans="1:61">
       <c r="A35" s="11">
         <v>57</v>
       </c>
@@ -7231,10 +7366,9 @@
       <c r="AS35" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="BI35" s="7"/>
-      <c r="BJ35" s="11"/>
-    </row>
-    <row r="36" spans="1:62">
+      <c r="BI35" s="11"/>
+    </row>
+    <row r="36" spans="1:61">
       <c r="A36" s="11">
         <v>78</v>
       </c>
@@ -7314,10 +7448,9 @@
       <c r="BG36" s="1">
         <v>1</v>
       </c>
-      <c r="BI36" s="7"/>
-      <c r="BJ36" s="11"/>
-    </row>
-    <row r="37" spans="1:62">
+      <c r="BI36" s="11"/>
+    </row>
+    <row r="37" spans="1:61">
       <c r="A37" s="11">
         <v>64</v>
       </c>
@@ -7384,10 +7517,9 @@
       <c r="BE37" s="1">
         <v>1</v>
       </c>
-      <c r="BI37" s="7"/>
-      <c r="BJ37" s="11"/>
-    </row>
-    <row r="38" spans="1:62">
+      <c r="BI37" s="11"/>
+    </row>
+    <row r="38" spans="1:61">
       <c r="A38" s="11">
         <v>68</v>
       </c>
@@ -7508,9 +7640,11 @@
       <c r="AO38" s="1">
         <v>75.2</v>
       </c>
-      <c r="BJ38" s="11"/>
-    </row>
-    <row r="39" spans="1:62">
+      <c r="BI38" s="11" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="39" spans="1:61">
       <c r="A39" s="11">
         <v>93</v>
       </c>
@@ -7580,10 +7714,9 @@
       <c r="BE39" s="1">
         <v>1</v>
       </c>
-      <c r="BI39" s="7"/>
-      <c r="BJ39" s="11"/>
-    </row>
-    <row r="40" spans="1:62">
+      <c r="BI39" s="11"/>
+    </row>
+    <row r="40" spans="1:61">
       <c r="A40" s="11">
         <v>48</v>
       </c>
@@ -7650,10 +7783,9 @@
       <c r="BG40" s="1">
         <v>1</v>
       </c>
-      <c r="BI40" s="7"/>
-      <c r="BJ40" s="11"/>
-    </row>
-    <row r="41" spans="1:62">
+      <c r="BI40" s="11"/>
+    </row>
+    <row r="41" spans="1:61">
       <c r="A41" s="11">
         <v>48</v>
       </c>
@@ -7699,10 +7831,9 @@
       <c r="U41" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="BI41" s="7"/>
-      <c r="BJ41" s="11"/>
-    </row>
-    <row r="42" spans="1:62" s="11" customFormat="1">
+      <c r="BI41" s="11"/>
+    </row>
+    <row r="42" spans="1:61" s="11" customFormat="1">
       <c r="A42" s="11">
         <v>88</v>
       </c>
@@ -7807,7 +7938,7 @@
       </c>
       <c r="AK42" s="14"/>
     </row>
-    <row r="43" spans="1:62" s="11" customFormat="1">
+    <row r="43" spans="1:61" s="11" customFormat="1">
       <c r="A43" s="11">
         <v>111</v>
       </c>
@@ -7875,7 +8006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:62" s="11" customFormat="1">
+    <row r="44" spans="1:61" s="11" customFormat="1">
       <c r="A44" s="11">
         <v>111</v>
       </c>
@@ -7931,7 +8062,7 @@
       <c r="AQ44" s="12"/>
       <c r="AR44" s="12"/>
     </row>
-    <row r="45" spans="1:62" s="11" customFormat="1">
+    <row r="45" spans="1:61" s="11" customFormat="1">
       <c r="A45" s="11">
         <v>111</v>
       </c>
@@ -7987,7 +8118,7 @@
       <c r="AQ45" s="13"/>
       <c r="AR45" s="13"/>
     </row>
-    <row r="46" spans="1:62" s="11" customFormat="1">
+    <row r="46" spans="1:61" s="11" customFormat="1">
       <c r="A46" s="11">
         <v>111</v>
       </c>
@@ -8043,7 +8174,7 @@
       <c r="AQ46" s="12"/>
       <c r="AR46" s="12"/>
     </row>
-    <row r="47" spans="1:62" s="11" customFormat="1">
+    <row r="47" spans="1:61" s="11" customFormat="1">
       <c r="A47" s="11">
         <v>111</v>
       </c>
@@ -8099,7 +8230,7 @@
       <c r="AQ47" s="12"/>
       <c r="AR47" s="12"/>
     </row>
-    <row r="48" spans="1:62" s="11" customFormat="1">
+    <row r="48" spans="1:61" s="11" customFormat="1">
       <c r="A48" s="11">
         <v>56</v>
       </c>
@@ -8132,7 +8263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:62" s="11" customFormat="1">
+    <row r="49" spans="1:61" s="11" customFormat="1">
       <c r="A49" s="11">
         <v>82</v>
       </c>
@@ -8165,7 +8296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:62" s="11" customFormat="1">
+    <row r="50" spans="1:61" s="11" customFormat="1">
       <c r="A50" s="11">
         <v>104</v>
       </c>
@@ -8254,8 +8385,11 @@
         <v>0.16</v>
       </c>
       <c r="AK50" s="14"/>
-    </row>
-    <row r="51" spans="1:62" s="11" customFormat="1">
+      <c r="BI50" s="11" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="51" spans="1:61" s="11" customFormat="1">
       <c r="A51" s="11">
         <v>87</v>
       </c>
@@ -8288,7 +8422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:62" s="11" customFormat="1">
+    <row r="52" spans="1:61" s="11" customFormat="1">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -8385,8 +8519,11 @@
       <c r="AS52" s="7" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="53" spans="1:62" s="11" customFormat="1">
+      <c r="BI52" s="30" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:61" s="11" customFormat="1">
       <c r="A53" s="11">
         <v>67</v>
       </c>
@@ -8503,8 +8640,11 @@
       <c r="AS53" s="1"/>
       <c r="AT53" s="1"/>
       <c r="AU53" s="1"/>
-    </row>
-    <row r="54" spans="1:62">
+      <c r="BI53" s="11" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="54" spans="1:61">
       <c r="A54" s="11">
         <v>96</v>
       </c>
@@ -8581,9 +8721,11 @@
       <c r="AS54" s="1" t="s">
         <v>1126</v>
       </c>
-      <c r="BJ54" s="11"/>
-    </row>
-    <row r="55" spans="1:62">
+      <c r="BI54" s="11" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:61">
       <c r="A55" s="11">
         <v>98</v>
       </c>
@@ -8662,9 +8804,11 @@
       <c r="AI55" s="1">
         <v>0.12</v>
       </c>
-      <c r="BJ55" s="11"/>
-    </row>
-    <row r="56" spans="1:62">
+      <c r="BI55" s="11" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="56" spans="1:61">
       <c r="A56" s="11">
         <v>79</v>
       </c>
@@ -8731,10 +8875,9 @@
       <c r="BG56" s="1">
         <v>1</v>
       </c>
-      <c r="BI56" s="7"/>
-      <c r="BJ56" s="11"/>
-    </row>
-    <row r="57" spans="1:62">
+      <c r="BI56" s="11"/>
+    </row>
+    <row r="57" spans="1:61">
       <c r="A57" s="11">
         <v>79</v>
       </c>
@@ -8792,10 +8935,9 @@
       <c r="AV57" s="1">
         <v>45144</v>
       </c>
-      <c r="BI57" s="7"/>
-      <c r="BJ57" s="11"/>
-    </row>
-    <row r="58" spans="1:62">
+      <c r="BI57" s="11"/>
+    </row>
+    <row r="58" spans="1:61">
       <c r="A58" s="11">
         <v>79</v>
       </c>
@@ -8853,10 +8995,9 @@
       <c r="AV58" s="1">
         <v>16930</v>
       </c>
-      <c r="BI58" s="7"/>
-      <c r="BJ58" s="11"/>
-    </row>
-    <row r="59" spans="1:62">
+      <c r="BI58" s="11"/>
+    </row>
+    <row r="59" spans="1:61">
       <c r="A59" s="11">
         <v>79</v>
       </c>
@@ -8914,10 +9055,9 @@
       <c r="AV59" s="1">
         <v>13059</v>
       </c>
-      <c r="BI59" s="7"/>
-      <c r="BJ59" s="11"/>
-    </row>
-    <row r="60" spans="1:62">
+      <c r="BI59" s="11"/>
+    </row>
+    <row r="60" spans="1:61">
       <c r="A60" s="11">
         <v>41</v>
       </c>
@@ -8975,10 +9115,9 @@
       <c r="BG60" s="1">
         <v>1</v>
       </c>
-      <c r="BI60" s="7"/>
-      <c r="BJ60" s="11"/>
-    </row>
-    <row r="61" spans="1:62">
+      <c r="BI60" s="11"/>
+    </row>
+    <row r="61" spans="1:61">
       <c r="A61" s="7">
         <v>41</v>
       </c>
@@ -9028,9 +9167,8 @@
         <v>605</v>
       </c>
       <c r="BI61" s="7"/>
-      <c r="BJ61" s="7"/>
-    </row>
-    <row r="62" spans="1:62">
+    </row>
+    <row r="62" spans="1:61">
       <c r="A62" s="11">
         <v>106</v>
       </c>
@@ -9136,9 +9274,9 @@
       <c r="AJ62" s="7">
         <v>0.18</v>
       </c>
-      <c r="BJ62" s="11"/>
-    </row>
-    <row r="63" spans="1:62">
+      <c r="BI62" s="11"/>
+    </row>
+    <row r="63" spans="1:61">
       <c r="A63" s="11">
         <v>99</v>
       </c>
@@ -9229,9 +9367,11 @@
       <c r="AR63" s="26">
         <v>0.19961490000000001</v>
       </c>
-      <c r="BJ63" s="11"/>
-    </row>
-    <row r="64" spans="1:62">
+      <c r="BI63" s="11" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="64" spans="1:61">
       <c r="A64" s="11">
         <v>94</v>
       </c>
@@ -9301,10 +9441,9 @@
       <c r="BE64" s="1">
         <v>1</v>
       </c>
-      <c r="BI64" s="7"/>
-      <c r="BJ64" s="11"/>
-    </row>
-    <row r="65" spans="1:62">
+      <c r="BI64" s="11"/>
+    </row>
+    <row r="65" spans="1:61">
       <c r="A65" s="11">
         <v>51</v>
       </c>
@@ -9336,9 +9475,9 @@
       <c r="BC65" s="1">
         <v>1</v>
       </c>
-      <c r="BJ65" s="11"/>
-    </row>
-    <row r="66" spans="1:62">
+      <c r="BI65" s="11"/>
+    </row>
+    <row r="66" spans="1:61">
       <c r="A66" s="11">
         <v>95</v>
       </c>
@@ -9370,10 +9509,9 @@
       <c r="BF66" s="1">
         <v>1</v>
       </c>
-      <c r="BI66" s="7"/>
-      <c r="BJ66" s="11"/>
-    </row>
-    <row r="67" spans="1:62">
+      <c r="BI66" s="11"/>
+    </row>
+    <row r="67" spans="1:61">
       <c r="A67" s="11">
         <v>85</v>
       </c>
@@ -9414,10 +9552,9 @@
       <c r="BE67" s="1">
         <v>1</v>
       </c>
-      <c r="BI67" s="7"/>
-      <c r="BJ67" s="11"/>
-    </row>
-    <row r="68" spans="1:62">
+      <c r="BI67" s="11"/>
+    </row>
+    <row r="68" spans="1:61">
       <c r="A68" s="11">
         <v>110</v>
       </c>
@@ -9445,10 +9582,9 @@
       <c r="BD68" s="1">
         <v>1</v>
       </c>
-      <c r="BI68" s="7"/>
-      <c r="BJ68" s="11"/>
-    </row>
-    <row r="69" spans="1:62">
+      <c r="BI68" s="11"/>
+    </row>
+    <row r="69" spans="1:61">
       <c r="A69" s="11">
         <v>73</v>
       </c>
@@ -9521,9 +9657,9 @@
       <c r="AS69" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="BJ69" s="11"/>
-    </row>
-    <row r="70" spans="1:62">
+      <c r="BI69" s="11"/>
+    </row>
+    <row r="70" spans="1:61">
       <c r="A70" s="7">
         <v>73</v>
       </c>
@@ -9593,9 +9729,9 @@
       <c r="BD70" s="1">
         <v>1</v>
       </c>
-      <c r="BJ70" s="7"/>
-    </row>
-    <row r="71" spans="1:62">
+      <c r="BI70" s="7"/>
+    </row>
+    <row r="71" spans="1:61">
       <c r="A71" s="11">
         <v>80</v>
       </c>
@@ -9623,10 +9759,9 @@
       <c r="BF71" s="1">
         <v>1</v>
       </c>
-      <c r="BI71" s="7"/>
-      <c r="BJ71" s="11"/>
-    </row>
-    <row r="72" spans="1:62">
+      <c r="BI71" s="11"/>
+    </row>
+    <row r="72" spans="1:61">
       <c r="A72" s="11">
         <v>52</v>
       </c>
@@ -9654,10 +9789,9 @@
       <c r="BE72" s="1">
         <v>1</v>
       </c>
-      <c r="BI72" s="7"/>
-      <c r="BJ72" s="11"/>
-    </row>
-    <row r="73" spans="1:62">
+      <c r="BI72" s="11"/>
+    </row>
+    <row r="73" spans="1:61">
       <c r="A73" s="11">
         <v>83</v>
       </c>
@@ -9727,10 +9861,9 @@
       <c r="BG73" s="1">
         <v>1</v>
       </c>
-      <c r="BI73" s="7"/>
-      <c r="BJ73" s="11"/>
-    </row>
-    <row r="74" spans="1:62">
+      <c r="BI73" s="11"/>
+    </row>
+    <row r="74" spans="1:61">
       <c r="A74" s="11">
         <v>91</v>
       </c>
@@ -9806,9 +9939,11 @@
       <c r="AJ74" s="1">
         <v>0.189</v>
       </c>
-      <c r="BJ74" s="11"/>
-    </row>
-    <row r="75" spans="1:62">
+      <c r="BI74" s="11" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="75" spans="1:61">
       <c r="A75" s="11">
         <v>72</v>
       </c>
@@ -9926,9 +10061,11 @@
       <c r="BB75" s="1">
         <v>0.999</v>
       </c>
-      <c r="BJ75" s="11"/>
-    </row>
-    <row r="76" spans="1:62">
+      <c r="BI75" s="11" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="76" spans="1:61">
       <c r="A76" s="11">
         <v>92</v>
       </c>
@@ -9998,9 +10135,11 @@
       <c r="AG76" s="7">
         <v>0.89</v>
       </c>
-      <c r="BJ76" s="11"/>
-    </row>
-    <row r="77" spans="1:62">
+      <c r="BI76" s="11" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="77" spans="1:61">
       <c r="A77" s="11">
         <v>58</v>
       </c>
@@ -10028,10 +10167,9 @@
       <c r="BE77" s="1">
         <v>1</v>
       </c>
-      <c r="BI77" s="7"/>
-      <c r="BJ77" s="11"/>
-    </row>
-    <row r="78" spans="1:62">
+      <c r="BI77" s="11"/>
+    </row>
+    <row r="78" spans="1:61">
       <c r="A78" s="11">
         <v>44</v>
       </c>
@@ -10137,9 +10275,11 @@
       <c r="AJ78" s="7">
         <v>0.18</v>
       </c>
-      <c r="BJ78" s="11"/>
-    </row>
-    <row r="79" spans="1:62">
+      <c r="BI78" s="11" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="79" spans="1:61">
       <c r="A79" s="11">
         <v>55</v>
       </c>
@@ -10167,10 +10307,9 @@
       <c r="BD79" s="1">
         <v>1</v>
       </c>
-      <c r="BI79" s="7"/>
-      <c r="BJ79" s="11"/>
-    </row>
-    <row r="80" spans="1:62">
+      <c r="BI79" s="11"/>
+    </row>
+    <row r="80" spans="1:61">
       <c r="A80" s="11">
         <v>43</v>
       </c>
@@ -10198,10 +10337,9 @@
       <c r="BE80" s="1">
         <v>1</v>
       </c>
-      <c r="BI80" s="7"/>
-      <c r="BJ80" s="11"/>
-    </row>
-    <row r="81" spans="1:62">
+      <c r="BI80" s="11"/>
+    </row>
+    <row r="81" spans="1:61">
       <c r="A81" s="11">
         <v>40</v>
       </c>
@@ -10310,9 +10448,11 @@
       <c r="BB81" s="1">
         <v>1</v>
       </c>
-      <c r="BJ81" s="11"/>
-    </row>
-    <row r="82" spans="1:62">
+      <c r="BI81" s="11" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="82" spans="1:61">
       <c r="A82" s="11">
         <v>81</v>
       </c>
@@ -10367,10 +10507,9 @@
       <c r="BG82" s="1">
         <v>1</v>
       </c>
-      <c r="BI82" s="7"/>
-      <c r="BJ82" s="11"/>
-    </row>
-    <row r="83" spans="1:62">
+      <c r="BI82" s="11"/>
+    </row>
+    <row r="83" spans="1:61">
       <c r="A83" s="7">
         <v>81</v>
       </c>
@@ -10417,9 +10556,8 @@
         <v>78041</v>
       </c>
       <c r="BI83" s="7"/>
-      <c r="BJ83" s="7"/>
-    </row>
-    <row r="84" spans="1:62">
+    </row>
+    <row r="84" spans="1:61">
       <c r="A84" s="11">
         <v>59</v>
       </c>
@@ -10504,9 +10642,11 @@
       <c r="AT84" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="BJ84" s="11"/>
-    </row>
-    <row r="85" spans="1:62">
+      <c r="BI84" s="11" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="85" spans="1:61">
       <c r="A85">
         <v>108</v>
       </c>
@@ -10561,9 +10701,9 @@
       <c r="BE85" s="1">
         <v>1</v>
       </c>
-      <c r="BJ85"/>
-    </row>
-    <row r="86" spans="1:62">
+      <c r="BI85"/>
+    </row>
+    <row r="86" spans="1:61">
       <c r="A86">
         <v>105</v>
       </c>
@@ -10591,9 +10731,9 @@
       <c r="BC86" s="1">
         <v>1</v>
       </c>
-      <c r="BJ86"/>
-    </row>
-    <row r="87" spans="1:62">
+      <c r="BI86"/>
+    </row>
+    <row r="87" spans="1:61">
       <c r="A87">
         <v>62</v>
       </c>
@@ -10674,9 +10814,11 @@
       <c r="AT87" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="BJ87"/>
-    </row>
-    <row r="88" spans="1:62">
+      <c r="BI87" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="88" spans="1:61">
       <c r="A88">
         <v>101</v>
       </c>
@@ -10704,9 +10846,9 @@
       <c r="BC88" s="1">
         <v>1</v>
       </c>
-      <c r="BJ88"/>
-    </row>
-    <row r="89" spans="1:62">
+      <c r="BI88"/>
+    </row>
+    <row r="89" spans="1:61">
       <c r="A89">
         <v>76</v>
       </c>
@@ -10779,9 +10921,9 @@
       <c r="BG89" s="1">
         <v>1</v>
       </c>
-      <c r="BJ89"/>
-    </row>
-    <row r="90" spans="1:62">
+      <c r="BI89"/>
+    </row>
+    <row r="90" spans="1:61">
       <c r="A90">
         <v>76</v>
       </c>
@@ -10848,9 +10990,9 @@
       <c r="AV90" s="1">
         <v>132</v>
       </c>
-      <c r="BJ90"/>
-    </row>
-    <row r="91" spans="1:62">
+      <c r="BI90"/>
+    </row>
+    <row r="91" spans="1:61">
       <c r="A91">
         <v>76</v>
       </c>
@@ -10917,9 +11059,9 @@
       <c r="AV91" s="1">
         <v>278</v>
       </c>
-      <c r="BJ91"/>
-    </row>
-    <row r="92" spans="1:62">
+      <c r="BI91"/>
+    </row>
+    <row r="92" spans="1:61">
       <c r="A92">
         <v>76</v>
       </c>
@@ -10986,9 +11128,9 @@
       <c r="AV92" s="1">
         <v>55</v>
       </c>
-      <c r="BJ92"/>
-    </row>
-    <row r="93" spans="1:62">
+      <c r="BI92"/>
+    </row>
+    <row r="93" spans="1:61">
       <c r="A93">
         <v>76</v>
       </c>
@@ -11052,9 +11194,9 @@
       <c r="AV93" s="1">
         <v>74</v>
       </c>
-      <c r="BJ93"/>
-    </row>
-    <row r="94" spans="1:62">
+      <c r="BI93"/>
+    </row>
+    <row r="94" spans="1:61">
       <c r="A94">
         <v>76</v>
       </c>
@@ -11121,9 +11263,9 @@
       <c r="AV94" s="1">
         <v>128</v>
       </c>
-      <c r="BJ94"/>
-    </row>
-    <row r="95" spans="1:62">
+      <c r="BI94"/>
+    </row>
+    <row r="95" spans="1:61">
       <c r="A95">
         <v>76</v>
       </c>
@@ -11190,9 +11332,9 @@
       <c r="AV95" s="1">
         <v>887</v>
       </c>
-      <c r="BJ95"/>
-    </row>
-    <row r="96" spans="1:62">
+      <c r="BI95"/>
+    </row>
+    <row r="96" spans="1:61">
       <c r="A96">
         <v>42</v>
       </c>
@@ -11292,9 +11434,11 @@
       <c r="AT96" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="BJ96"/>
-    </row>
-    <row r="97" spans="1:62">
+      <c r="BI96" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="97" spans="1:61">
       <c r="A97">
         <v>89</v>
       </c>
@@ -11364,9 +11508,11 @@
       <c r="AG97" s="7">
         <v>0.98</v>
       </c>
-      <c r="BJ97"/>
-    </row>
-    <row r="98" spans="1:62">
+      <c r="BI97" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="98" spans="1:61">
       <c r="A98">
         <v>50</v>
       </c>
@@ -11493,9 +11639,9 @@
       <c r="BB98" s="1">
         <v>0.95</v>
       </c>
-      <c r="BJ98"/>
-    </row>
-    <row r="99" spans="1:62">
+      <c r="BI98"/>
+    </row>
+    <row r="99" spans="1:61">
       <c r="A99" s="1">
         <v>50</v>
       </c>
@@ -11614,7 +11760,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="100" spans="1:62">
+    <row r="100" spans="1:61">
       <c r="A100">
         <v>112</v>
       </c>
@@ -11690,9 +11836,11 @@
       <c r="AJ100" s="7">
         <v>0.19</v>
       </c>
-      <c r="BJ100"/>
-    </row>
-    <row r="101" spans="1:62">
+      <c r="BI100" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="101" spans="1:61">
       <c r="A101" s="1">
         <v>112</v>
       </c>
@@ -11760,7 +11908,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="102" spans="1:62">
+    <row r="102" spans="1:61">
       <c r="A102">
         <v>70</v>
       </c>
@@ -11827,9 +11975,9 @@
       <c r="BE102" s="1">
         <v>1</v>
       </c>
-      <c r="BJ102"/>
-    </row>
-    <row r="103" spans="1:62">
+      <c r="BI102"/>
+    </row>
+    <row r="103" spans="1:61">
       <c r="A103">
         <v>47</v>
       </c>
@@ -11854,9 +12002,9 @@
       <c r="BD103" s="1">
         <v>1</v>
       </c>
-      <c r="BJ103"/>
-    </row>
-    <row r="104" spans="1:62">
+      <c r="BI103"/>
+    </row>
+    <row r="104" spans="1:61">
       <c r="A104">
         <v>103</v>
       </c>
@@ -11971,9 +12119,11 @@
       <c r="AT104" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="BJ104"/>
-    </row>
-    <row r="105" spans="1:62">
+      <c r="BI104" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="105" spans="1:61">
       <c r="A105">
         <v>97</v>
       </c>
@@ -12064,9 +12214,11 @@
       <c r="AT105" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="BJ105"/>
-    </row>
-    <row r="106" spans="1:62">
+      <c r="BI105" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="106" spans="1:61">
       <c r="A106">
         <v>65</v>
       </c>
@@ -12214,9 +12366,11 @@
       <c r="BB106" s="1">
         <v>0.99</v>
       </c>
-      <c r="BJ106"/>
-    </row>
-    <row r="107" spans="1:62">
+      <c r="BI106" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="107" spans="1:61">
       <c r="A107" s="11">
         <v>113</v>
       </c>
@@ -12290,9 +12444,11 @@
       <c r="AT107" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="BJ107" s="11"/>
-    </row>
-    <row r="108" spans="1:62">
+      <c r="BI107" s="11" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="108" spans="1:61">
       <c r="A108" s="11">
         <v>118</v>
       </c>
@@ -12377,9 +12533,11 @@
       <c r="AJ108" s="7">
         <v>0.1</v>
       </c>
-      <c r="BJ108" s="11"/>
-    </row>
-    <row r="109" spans="1:62">
+      <c r="BI108" s="11" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="109" spans="1:61">
       <c r="A109" s="11">
         <v>118</v>
       </c>
@@ -12461,9 +12619,9 @@
       <c r="AT109" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="BJ109" s="7"/>
-    </row>
-    <row r="110" spans="1:62">
+      <c r="BI109" s="7"/>
+    </row>
+    <row r="110" spans="1:61">
       <c r="A110" s="11">
         <v>121</v>
       </c>
@@ -12548,9 +12706,11 @@
       <c r="AT110" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="BJ110" s="11"/>
-    </row>
-    <row r="111" spans="1:62">
+      <c r="BI110" s="11" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="111" spans="1:61">
       <c r="A111" s="11">
         <v>115</v>
       </c>
@@ -12632,9 +12792,11 @@
       <c r="AT111" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="BJ111" s="11"/>
-    </row>
-    <row r="112" spans="1:62">
+      <c r="BI111" s="11" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="112" spans="1:61">
       <c r="A112" s="11">
         <v>117</v>
       </c>
@@ -12734,9 +12896,11 @@
       <c r="AT112" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="BJ112" s="11"/>
-    </row>
-    <row r="113" spans="1:62">
+      <c r="BI112" s="11" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="113" spans="1:61">
       <c r="A113" s="11">
         <v>116</v>
       </c>
@@ -12845,9 +13009,11 @@
       <c r="AT113" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="BJ113" s="11"/>
-    </row>
-    <row r="114" spans="1:62">
+      <c r="BI113" s="11" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="114" spans="1:61">
       <c r="A114" s="11">
         <v>123</v>
       </c>
@@ -12929,9 +13095,11 @@
       <c r="AT114" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="BJ114" s="11"/>
-    </row>
-    <row r="115" spans="1:62">
+      <c r="BI114" s="11" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="115" spans="1:61">
       <c r="A115" s="11">
         <v>119</v>
       </c>
@@ -13025,9 +13193,11 @@
       <c r="AT115" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="BJ115" s="11"/>
-    </row>
-    <row r="116" spans="1:62">
+      <c r="BI115" s="11" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="116" spans="1:61">
       <c r="A116" s="11">
         <v>114</v>
       </c>
@@ -13116,9 +13286,9 @@
       <c r="AT116" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="BJ116" s="11"/>
-    </row>
-    <row r="117" spans="1:62">
+      <c r="BI116" s="11"/>
+    </row>
+    <row r="117" spans="1:61">
       <c r="A117" s="11">
         <v>114</v>
       </c>
@@ -13198,9 +13368,9 @@
       <c r="AS117" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="BJ117" s="11"/>
-    </row>
-    <row r="118" spans="1:62">
+      <c r="BI117" s="11"/>
+    </row>
+    <row r="118" spans="1:61">
       <c r="A118" s="11">
         <v>114</v>
       </c>
@@ -13280,9 +13450,9 @@
       <c r="AS118" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="BJ118" s="11"/>
-    </row>
-    <row r="119" spans="1:62">
+      <c r="BI118" s="11"/>
+    </row>
+    <row r="119" spans="1:61">
       <c r="A119" s="7">
         <v>114</v>
       </c>
@@ -13362,9 +13532,9 @@
       <c r="AS119" s="1" t="s">
         <v>1166</v>
       </c>
-      <c r="BJ119" s="7"/>
-    </row>
-    <row r="120" spans="1:62">
+      <c r="BI119" s="7"/>
+    </row>
+    <row r="120" spans="1:61">
       <c r="A120" s="11">
         <v>122</v>
       </c>
@@ -13437,9 +13607,9 @@
       <c r="AT120" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="BJ120" s="11"/>
-    </row>
-    <row r="121" spans="1:62">
+      <c r="BI120" s="11"/>
+    </row>
+    <row r="121" spans="1:61">
       <c r="A121" s="11">
         <v>120</v>
       </c>
@@ -13485,10 +13655,9 @@
       <c r="BE121" s="1">
         <v>1</v>
       </c>
-      <c r="BI121" s="7"/>
-      <c r="BJ121" s="11"/>
-    </row>
-    <row r="122" spans="1:62">
+      <c r="BI121" s="11"/>
+    </row>
+    <row r="122" spans="1:61">
       <c r="A122">
         <v>129</v>
       </c>
@@ -13576,9 +13745,11 @@
       <c r="AT122" s="1" t="s">
         <v>968</v>
       </c>
-      <c r="BJ122"/>
-    </row>
-    <row r="123" spans="1:62">
+      <c r="BI122" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="123" spans="1:61">
       <c r="A123">
         <v>126</v>
       </c>
@@ -13684,9 +13855,11 @@
       <c r="AT123" s="1" t="s">
         <v>971</v>
       </c>
-      <c r="BJ123"/>
-    </row>
-    <row r="124" spans="1:62">
+      <c r="BI123" s="11" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="124" spans="1:61">
       <c r="A124">
         <v>124</v>
       </c>
@@ -13780,9 +13953,11 @@
       <c r="AT124" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="BJ124"/>
-    </row>
-    <row r="125" spans="1:62">
+      <c r="BI124" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="125" spans="1:61">
       <c r="A125">
         <v>131</v>
       </c>
@@ -13867,9 +14042,11 @@
       <c r="AT125" s="1" t="s">
         <v>983</v>
       </c>
-      <c r="BJ125"/>
-    </row>
-    <row r="126" spans="1:62">
+      <c r="BI125" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="126" spans="1:61">
       <c r="A126">
         <v>125</v>
       </c>
@@ -13960,9 +14137,11 @@
       <c r="AT126" s="1" t="s">
         <v>987</v>
       </c>
-      <c r="BJ126"/>
-    </row>
-    <row r="127" spans="1:62">
+      <c r="BI126" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="127" spans="1:61">
       <c r="A127">
         <v>127</v>
       </c>
@@ -14050,9 +14229,9 @@
       <c r="AT127" s="1" t="s">
         <v>993</v>
       </c>
-      <c r="BJ127"/>
-    </row>
-    <row r="128" spans="1:62">
+      <c r="BI127"/>
+    </row>
+    <row r="128" spans="1:61">
       <c r="A128">
         <v>129</v>
       </c>
@@ -14089,178 +14268,181 @@
       <c r="BH128" s="1">
         <v>1</v>
       </c>
-      <c r="BJ128"/>
+      <c r="BI128"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="BI52" r:id="rId1" xr:uid="{86F6EA99-076A-4817-8DA8-2862D1AA3B05}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E6D177-A1E6-4E78-B3F8-6755B06A4B81}">
-  <dimension ref="A1:AP61"/>
+  <dimension ref="A1:AI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="92" workbookViewId="0">
-      <selection activeCell="B61" sqref="B2:B61"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:42" s="1" customFormat="1">
+    <row r="1" spans="1:35" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>1000</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1001</v>
       </c>
-      <c r="R1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="7"/>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
-      <c r="U1" s="8"/>
+      <c r="U1" s="7"/>
       <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AG1" s="9"/>
-      <c r="AL1" s="4"/>
-    </row>
-    <row r="2" spans="1:42" s="1" customFormat="1">
+      <c r="Z1" s="9"/>
+      <c r="AE1" s="4"/>
+    </row>
+    <row r="2" spans="1:35" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>401</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>1001</v>
-      </c>
-      <c r="R2" s="8"/>
+        <v>1002</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
-      <c r="U2" s="8"/>
+      <c r="U2" s="7"/>
       <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AG2" s="9"/>
-      <c r="AP2" s="4"/>
-    </row>
-    <row r="3" spans="1:42">
+      <c r="Z2" s="9"/>
+      <c r="AI2" s="4"/>
+    </row>
+    <row r="3" spans="1:35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
       <c r="A7" s="1" t="s">
         <v>417</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
       <c r="A9" s="1" t="s">
         <v>1071</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
       <c r="A11" s="1" t="s">
         <v>1010</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="14" spans="1:42">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:42">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35">
       <c r="A15" s="1" t="s">
         <v>476</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35">
       <c r="A16" s="1" t="s">
-        <v>398</v>
+        <v>1300</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>1254</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -14268,7 +14450,7 @@
         <v>391</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>1018</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -14276,7 +14458,7 @@
         <v>390</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -14284,7 +14466,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -14292,7 +14474,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>1011</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -14300,7 +14482,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -14308,7 +14490,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -14316,7 +14498,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -14324,7 +14506,7 @@
         <v>1023</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>1022</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -14332,7 +14514,7 @@
         <v>1027</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -14340,7 +14522,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -14348,7 +14530,7 @@
         <v>1024</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -14356,7 +14538,7 @@
         <v>1028</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>1031</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -14364,7 +14546,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -14372,7 +14554,7 @@
         <v>1025</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -14380,7 +14562,7 @@
         <v>1029</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -14388,137 +14570,135 @@
         <v>14</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="87">
       <c r="A35" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B35" s="27" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="90">
+      <c r="B35" s="28" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="B36" s="27" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>385</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>1044</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>1026</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>389</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>1162</v>
       </c>
-      <c r="B43" s="27" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="B43" s="29" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>1163</v>
       </c>
-      <c r="B44" s="27" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="B44" s="29" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>1164</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="29" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="B46" s="27" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B47" s="29" t="s">
-        <v>1257</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="B47" s="27" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>684</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -14526,7 +14706,7 @@
         <v>685</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -14534,7 +14714,7 @@
         <v>682</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -14542,7 +14722,7 @@
         <v>683</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -14550,7 +14730,7 @@
         <v>686</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -14558,7 +14738,7 @@
         <v>687</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -14566,7 +14746,7 @@
         <v>688</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -14574,7 +14754,7 @@
         <v>689</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -14582,7 +14762,7 @@
         <v>1062</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>1058</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -14590,7 +14770,7 @@
         <v>1063</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -14598,7 +14778,7 @@
         <v>1064</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>1259</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -14606,7 +14786,7 @@
         <v>1065</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -14614,7 +14794,7 @@
         <v>1066</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -14622,7 +14802,7 @@
         <v>1067</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>1059</v>
+        <v>1299</v>
       </c>
     </row>
   </sheetData>
@@ -14639,7 +14819,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="19" t="s">
@@ -15564,11 +15744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09C1A9C-0E98-41EC-90F4-5B4D4F187A41}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A2:B11"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -15668,15 +15848,15 @@
       <selection activeCell="B2" sqref="B2:B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="66.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="66.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18050,7 +18230,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A77:J87">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A77:J87">
     <sortCondition ref="J77:J87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18066,7 +18246,7 @@
       <selection activeCell="B12" activeCellId="1" sqref="B15:B21 B2:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="11" t="s">
@@ -18415,7 +18595,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A15:D21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:D21">
     <sortCondition ref="D15:D21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18431,7 +18611,7 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="19" t="s">
@@ -18665,7 +18845,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
     <sortCondition ref="B2:B21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18681,9 +18861,9 @@
       <selection activeCell="B1" sqref="B1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>